<commit_message>
work 1.1.3 Week report with miss
</commit_message>
<xml_diff>
--- a/files_samples/Статистика операторов с пропущенными.xlsx
+++ b/files_samples/Статистика операторов с пропущенными.xlsx
@@ -179,7 +179,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="47">
+  <fills count="48">
     <fill>
       <patternFill/>
     </fill>
@@ -448,6 +448,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00C00000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC000"/>
       </patternFill>
     </fill>
   </fills>
@@ -764,7 +769,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -829,6 +834,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="46" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="47" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1310,7 +1318,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Пятница, 25.10.2024</t>
+          <t>Среда, 13.11.2024</t>
         </is>
       </c>
       <c r="B1" s="16" t="n"/>
@@ -1390,30 +1398,30 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>Архангельская Елена Николаевна</t>
+          <t>Абдулина Дарья Игоревна</t>
         </is>
       </c>
       <c r="B3" s="18" t="n">
-        <v>25</v>
-      </c>
-      <c r="C3" s="19" t="inlineStr">
-        <is>
-          <t>192</t>
+        <v>9</v>
+      </c>
+      <c r="C3" s="22" t="inlineStr">
+        <is>
+          <t>294</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>2:58:12</t>
+          <t>1:55:13</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>1:21:34</t>
+          <t>44:41</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>1:10:32</t>
+          <t>3:42</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
@@ -1436,12 +1444,12 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K3" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L3" s="10" t="n">
+      <c r="K3" s="21" t="inlineStr">
+        <is>
+          <t>4.83</t>
+        </is>
+      </c>
+      <c r="L3" s="19" t="n">
         <v>0</v>
       </c>
       <c r="M3" s="15" t="n"/>
@@ -1451,45 +1459,45 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>Баландин Дмитрий Алексеевич</t>
-        </is>
-      </c>
-      <c r="B4" s="18" t="n">
-        <v>19</v>
+          <t>Архангельская Елена Николаевна</t>
+        </is>
+      </c>
+      <c r="B4" s="19" t="n">
+        <v>68</v>
       </c>
       <c r="C4" s="19" t="inlineStr">
         <is>
-          <t>193</t>
+          <t>189</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>5:57:42</t>
+          <t>6:43:58</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>1:03:37</t>
+          <t>3:38:10</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>15:01</t>
+          <t>18:24</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>29:15</t>
         </is>
       </c>
       <c r="H4" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>10:08</t>
         </is>
       </c>
       <c r="I4" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>23:09</t>
         </is>
       </c>
       <c r="J4" s="3" t="inlineStr">
@@ -1497,13 +1505,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K4" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L4" s="13" t="n">
-        <v>7</v>
+      <c r="K4" s="21" t="inlineStr">
+        <is>
+          <t>4.80</t>
+        </is>
+      </c>
+      <c r="L4" s="19" t="n">
+        <v>0</v>
       </c>
       <c r="M4" s="15" t="n"/>
       <c r="P4" s="15" t="n"/>
@@ -1512,59 +1520,59 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Баринова София Андреевна</t>
-        </is>
-      </c>
-      <c r="B5" s="19" t="n">
-        <v>104</v>
-      </c>
-      <c r="C5" s="20" t="inlineStr">
-        <is>
-          <t>128</t>
+          <t>Баландин Дмитрий Алексеевич</t>
+        </is>
+      </c>
+      <c r="B5" s="18" t="n">
+        <v>16</v>
+      </c>
+      <c r="C5" s="23" t="inlineStr">
+        <is>
+          <t>437</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>5:08:48</t>
+          <t>5:57:56</t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>3:47:11</t>
+          <t>1:58:28</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>4:05</t>
+          <t>0:56</t>
         </is>
       </c>
       <c r="G5" s="3" t="inlineStr">
         <is>
-          <t>1:51</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="H5" s="3" t="inlineStr">
         <is>
-          <t>4:24</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I5" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>8:44</t>
         </is>
       </c>
       <c r="J5" s="3" t="inlineStr">
         <is>
-          <t>2:27:41</t>
-        </is>
-      </c>
-      <c r="K5" s="21" t="inlineStr">
-        <is>
-          <t>4.64</t>
-        </is>
-      </c>
-      <c r="L5" s="13" t="n">
-        <v>6</v>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="K5" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L5" s="21" t="n">
+        <v>5</v>
       </c>
       <c r="M5" s="15" t="n"/>
       <c r="P5" s="15" t="n"/>
@@ -1573,30 +1581,30 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Бахтиаров Глеб Русланович</t>
+          <t>Горных Ксения Сергеевна</t>
         </is>
       </c>
       <c r="B6" s="18" t="n">
-        <v>22</v>
-      </c>
-      <c r="C6" s="22" t="inlineStr">
-        <is>
-          <t>308</t>
+        <v>55</v>
+      </c>
+      <c r="C6" s="21" t="inlineStr">
+        <is>
+          <t>231</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>2:12:35</t>
+          <t>4:59:08</t>
         </is>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>1:53:47</t>
+          <t>3:36:47</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>15:49:29</t>
+          <t>1:31</t>
         </is>
       </c>
       <c r="G6" s="3" t="inlineStr">
@@ -1619,13 +1627,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K6" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L6" s="14" t="n">
-        <v>1</v>
+      <c r="K6" s="21" t="inlineStr">
+        <is>
+          <t>4.68</t>
+        </is>
+      </c>
+      <c r="L6" s="21" t="n">
+        <v>10</v>
       </c>
       <c r="M6" s="15" t="n"/>
       <c r="P6" s="15" t="n"/>
@@ -1634,40 +1642,40 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Гарипова Лейсан Миневелиевна</t>
-        </is>
-      </c>
-      <c r="B7" s="20" t="n">
-        <v>118</v>
-      </c>
-      <c r="C7" s="22" t="inlineStr">
-        <is>
-          <t>249</t>
+          <t>Гребенюк Полина Максимовна</t>
+        </is>
+      </c>
+      <c r="B7" s="18" t="n">
+        <v>25</v>
+      </c>
+      <c r="C7" s="21" t="inlineStr">
+        <is>
+          <t>224</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>11:08:43</t>
+          <t>2:16:19</t>
         </is>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>8:14:01</t>
+          <t>1:33:57</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>15:06</t>
+          <t>4:25</t>
         </is>
       </c>
       <c r="G7" s="3" t="inlineStr">
         <is>
-          <t>30:37</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="H7" s="3" t="inlineStr">
         <is>
-          <t>23:26</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I7" s="3" t="inlineStr">
@@ -1680,12 +1688,12 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K7" s="21" t="inlineStr">
-        <is>
-          <t>4.91</t>
-        </is>
-      </c>
-      <c r="L7" s="10" t="n">
+      <c r="K7" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L7" s="19" t="n">
         <v>0</v>
       </c>
       <c r="M7" s="15" t="n"/>
@@ -1695,45 +1703,45 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>Гарифуллин Булат Дамирович</t>
-        </is>
-      </c>
-      <c r="B8" s="19" t="n">
-        <v>94</v>
+          <t>Джабраилова Елена Валерьевна</t>
+        </is>
+      </c>
+      <c r="B8" s="20" t="n">
+        <v>148</v>
       </c>
       <c r="C8" s="19" t="inlineStr">
         <is>
-          <t>155</t>
+          <t>180</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>5:49:03</t>
+          <t>10:47:49</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>4:13:41</t>
+          <t>7:36:25</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>26:15</t>
+          <t>2:33</t>
         </is>
       </c>
       <c r="G8" s="3" t="inlineStr">
         <is>
-          <t>18:26</t>
+          <t>30:03</t>
         </is>
       </c>
       <c r="H8" s="3" t="inlineStr">
         <is>
-          <t>28:27</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I8" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>29:18</t>
         </is>
       </c>
       <c r="J8" s="3" t="inlineStr">
@@ -1741,13 +1749,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K8" s="21" t="inlineStr">
-        <is>
-          <t>4.78</t>
+      <c r="K8" s="22" t="inlineStr">
+        <is>
+          <t>4.70</t>
         </is>
       </c>
       <c r="L8" s="13" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="M8" s="15" t="n"/>
       <c r="P8" s="15" t="n"/>
@@ -1756,35 +1764,35 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>Горных Ксения Сергеевна</t>
+          <t>Довыдович Алиса Станиславовна</t>
         </is>
       </c>
       <c r="B9" s="18" t="n">
-        <v>60</v>
-      </c>
-      <c r="C9" s="21" t="inlineStr">
-        <is>
-          <t>213</t>
+        <v>32</v>
+      </c>
+      <c r="C9" s="19" t="inlineStr">
+        <is>
+          <t>177</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>4:42:09</t>
+          <t>1:59:50</t>
         </is>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>3:36:53</t>
+          <t>1:34:54</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>5:15:29</t>
+          <t>13:40</t>
         </is>
       </c>
       <c r="G9" s="3" t="inlineStr">
         <is>
-          <t>0:01</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="H9" s="3" t="inlineStr">
@@ -1802,13 +1810,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K9" s="21" t="inlineStr">
-        <is>
-          <t>4.90</t>
-        </is>
-      </c>
-      <c r="L9" s="13" t="n">
-        <v>10</v>
+      <c r="K9" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L9" s="19" t="n">
+        <v>0</v>
       </c>
       <c r="M9" s="15" t="n"/>
       <c r="Q9" s="15" t="n"/>
@@ -1816,30 +1824,30 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>Гребенюк Полина Максимовна</t>
+          <t>Егоров Олег Александрович</t>
         </is>
       </c>
       <c r="B10" s="18" t="n">
-        <v>37</v>
-      </c>
-      <c r="C10" s="23" t="inlineStr">
-        <is>
-          <t>373</t>
+        <v>45</v>
+      </c>
+      <c r="C10" s="20" t="inlineStr">
+        <is>
+          <t>140</t>
         </is>
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>6:05:48</t>
+          <t>1:44:38</t>
         </is>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>3:51:34</t>
+          <t>1:45:22</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>3:00</t>
+          <t>10:19:38</t>
         </is>
       </c>
       <c r="G10" s="3" t="inlineStr">
@@ -1849,7 +1857,7 @@
       </c>
       <c r="H10" s="3" t="inlineStr">
         <is>
-          <t>5:24</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I10" s="3" t="inlineStr">
@@ -1862,12 +1870,12 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K10" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L10" s="13" t="n">
+      <c r="K10" s="21" t="inlineStr">
+        <is>
+          <t>4.89</t>
+        </is>
+      </c>
+      <c r="L10" s="21" t="n">
         <v>2</v>
       </c>
       <c r="M10" s="15" t="n"/>
@@ -1877,40 +1885,40 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Джабраилова Елена Валерьевна</t>
+          <t>Жданов Денис Александрович</t>
         </is>
       </c>
       <c r="B11" s="18" t="n">
-        <v>90</v>
-      </c>
-      <c r="C11" s="19" t="inlineStr">
-        <is>
-          <t>169</t>
+        <v>56</v>
+      </c>
+      <c r="C11" s="22" t="inlineStr">
+        <is>
+          <t>268</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>7:51:36</t>
+          <t>4:43:23</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>4:21:11</t>
+          <t>4:13:22</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>2:13</t>
+          <t>5:07</t>
         </is>
       </c>
       <c r="G11" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>0:08</t>
         </is>
       </c>
       <c r="H11" s="3" t="inlineStr">
         <is>
-          <t>8:44</t>
+          <t>4:51</t>
         </is>
       </c>
       <c r="I11" s="3" t="inlineStr">
@@ -1920,15 +1928,15 @@
       </c>
       <c r="J11" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
-        </is>
-      </c>
-      <c r="K11" s="21" t="inlineStr">
-        <is>
-          <t>4.63</t>
-        </is>
-      </c>
-      <c r="L11" s="10" t="n">
+          <t>16:13</t>
+        </is>
+      </c>
+      <c r="K11" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L11" s="19" t="n">
         <v>0</v>
       </c>
       <c r="M11" s="15" t="n"/>
@@ -1938,30 +1946,30 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>Егоров Олег Александрович</t>
+          <t>Жевнер Григорий Павлович</t>
         </is>
       </c>
       <c r="B12" s="18" t="n">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C12" s="20" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>136</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>1:08:13</t>
+          <t>3:03:56</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>1:15:55</t>
+          <t>32:03</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>10:46:05</t>
+          <t>46:28</t>
         </is>
       </c>
       <c r="G12" s="3" t="inlineStr">
@@ -1984,12 +1992,12 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K12" s="21" t="inlineStr">
-        <is>
-          <t>4.76</t>
-        </is>
-      </c>
-      <c r="L12" s="10" t="n">
+      <c r="K12" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L12" s="19" t="n">
         <v>0</v>
       </c>
       <c r="M12" s="15" t="n"/>
@@ -1999,30 +2007,30 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Жданов Денис Александрович</t>
+          <t>Зиберт Ольга Николаевна</t>
         </is>
       </c>
       <c r="B13" s="18" t="n">
-        <v>83</v>
-      </c>
-      <c r="C13" s="22" t="inlineStr">
-        <is>
-          <t>270</t>
+        <v>24</v>
+      </c>
+      <c r="C13" s="23" t="inlineStr">
+        <is>
+          <t>434</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>7:59:10</t>
+          <t>3:25:13</t>
         </is>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>6:18:02</t>
+          <t>2:55:45</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>3:10</t>
+          <t>29:57</t>
         </is>
       </c>
       <c r="G13" s="3" t="inlineStr">
@@ -2032,7 +2040,7 @@
       </c>
       <c r="H13" s="3" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I13" s="3" t="inlineStr">
@@ -2047,11 +2055,11 @@
       </c>
       <c r="K13" s="21" t="inlineStr">
         <is>
-          <t>4.84</t>
-        </is>
-      </c>
-      <c r="L13" s="11" t="n">
-        <v>13</v>
+          <t>4.33</t>
+        </is>
+      </c>
+      <c r="L13" s="21" t="n">
+        <v>2</v>
       </c>
       <c r="M13" s="15" t="n"/>
       <c r="P13" s="15" t="n"/>
@@ -2060,35 +2068,35 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>Жевнер Григорий Павлович</t>
+          <t>Клочкова София Антоновна</t>
         </is>
       </c>
       <c r="B14" s="18" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C14" s="22" t="inlineStr">
         <is>
-          <t>241</t>
+          <t>295</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>11:14:44</t>
+          <t>2:08:15</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>57:41</t>
+          <t>1:49:05</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>51:33</t>
+          <t>42:42</t>
         </is>
       </c>
       <c r="G14" s="3" t="inlineStr">
         <is>
-          <t>8:32</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="H14" s="3" t="inlineStr">
@@ -2106,12 +2114,12 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K14" s="21" t="inlineStr">
-        <is>
-          <t>4.83</t>
-        </is>
-      </c>
-      <c r="L14" s="10" t="n">
+      <c r="K14" s="22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L14" s="19" t="n">
         <v>0</v>
       </c>
       <c r="M14" s="15" t="n"/>
@@ -2121,30 +2129,30 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>Идрисалиева Ольга Ивановна</t>
+          <t>Маркелов Сергей Алексеевич</t>
         </is>
       </c>
       <c r="B15" s="18" t="n">
-        <v>24</v>
-      </c>
-      <c r="C15" s="21" t="inlineStr">
-        <is>
-          <t>205</t>
+        <v>59</v>
+      </c>
+      <c r="C15" s="19" t="inlineStr">
+        <is>
+          <t>157</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>3:00:45</t>
+          <t>9:49:39</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>1:23:35</t>
+          <t>2:35:50</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>19:42</t>
+          <t>52:01</t>
         </is>
       </c>
       <c r="G15" s="3" t="inlineStr">
@@ -2154,7 +2162,7 @@
       </c>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>9:48</t>
         </is>
       </c>
       <c r="I15" s="3" t="inlineStr">
@@ -2164,16 +2172,16 @@
       </c>
       <c r="J15" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
-        </is>
-      </c>
-      <c r="K15" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L15" s="11" t="n">
-        <v>15</v>
+          <t>1:58:54</t>
+        </is>
+      </c>
+      <c r="K15" s="21" t="inlineStr">
+        <is>
+          <t>4.61</t>
+        </is>
+      </c>
+      <c r="L15" s="21" t="n">
+        <v>2</v>
       </c>
       <c r="M15" s="15" t="n"/>
       <c r="P15" s="15" t="n"/>
@@ -2182,30 +2190,30 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>Исаева Екатерина Аркадьевна</t>
+          <t>Матылицкая Елена Юрьевна</t>
         </is>
       </c>
       <c r="B16" s="18" t="n">
-        <v>28</v>
-      </c>
-      <c r="C16" s="21" t="inlineStr">
-        <is>
-          <t>208</t>
+        <v>26</v>
+      </c>
+      <c r="C16" s="22" t="inlineStr">
+        <is>
+          <t>285</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>2:11:50</t>
+          <t>2:58:13</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>1:42:05</t>
+          <t>2:05:25</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>1:15:47</t>
+          <t>34:05</t>
         </is>
       </c>
       <c r="G16" s="3" t="inlineStr">
@@ -2215,12 +2223,12 @@
       </c>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>7:32</t>
         </is>
       </c>
       <c r="I16" s="3" t="inlineStr">
         <is>
-          <t>5:17</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J16" s="3" t="inlineStr">
@@ -2230,11 +2238,11 @@
       </c>
       <c r="K16" s="21" t="inlineStr">
         <is>
-          <t>4.23</t>
-        </is>
-      </c>
-      <c r="L16" s="14" t="n">
-        <v>1</v>
+          <t>4.92</t>
+        </is>
+      </c>
+      <c r="L16" s="19" t="n">
+        <v>0</v>
       </c>
       <c r="M16" s="15" t="n"/>
       <c r="P16" s="15" t="n"/>
@@ -2243,30 +2251,30 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Куликов Максим Геннадьевич</t>
+          <t>Миргазова Ляйсан Ришатовна</t>
         </is>
       </c>
       <c r="B17" s="18" t="n">
-        <v>49</v>
-      </c>
-      <c r="C17" s="20" t="inlineStr">
-        <is>
-          <t>134</t>
+        <v>43</v>
+      </c>
+      <c r="C17" s="19" t="inlineStr">
+        <is>
+          <t>191</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>9:44:10</t>
+          <t>4:01:17</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>1:54:42</t>
+          <t>2:20:59</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>7:27</t>
+          <t>6:01</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
@@ -2276,7 +2284,7 @@
       </c>
       <c r="H17" s="3" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I17" s="3" t="inlineStr">
@@ -2286,16 +2294,16 @@
       </c>
       <c r="J17" s="3" t="inlineStr">
         <is>
-          <t>4:13</t>
-        </is>
-      </c>
-      <c r="K17" s="21" t="inlineStr">
-        <is>
-          <t>4.78</t>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="K17" s="22" t="inlineStr">
+        <is>
+          <t>4.46</t>
         </is>
       </c>
       <c r="L17" s="11" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M17" s="15" t="n"/>
       <c r="P17" s="15" t="n"/>
@@ -2304,30 +2312,30 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>Маркелов Сергей Алексеевич</t>
+          <t>Мунасипова Надия Мидхатовна</t>
         </is>
       </c>
       <c r="B18" s="18" t="n">
-        <v>57</v>
-      </c>
-      <c r="C18" s="19" t="inlineStr">
-        <is>
-          <t>160</t>
+        <v>10</v>
+      </c>
+      <c r="C18" s="23" t="inlineStr">
+        <is>
+          <t>616</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>6:19:06</t>
+          <t>2:06:24</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>2:33:09</t>
+          <t>1:43:26</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>49:54</t>
+          <t>1.06:54:14</t>
         </is>
       </c>
       <c r="G18" s="3" t="inlineStr">
@@ -2347,16 +2355,16 @@
       </c>
       <c r="J18" s="3" t="inlineStr">
         <is>
-          <t>2:00:09</t>
-        </is>
-      </c>
-      <c r="K18" s="21" t="inlineStr">
-        <is>
-          <t>4.68</t>
-        </is>
-      </c>
-      <c r="L18" s="11" t="n">
-        <v>16</v>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="K18" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L18" s="19" t="n">
+        <v>0</v>
       </c>
       <c r="M18" s="15" t="n"/>
       <c r="P18" s="15" t="n"/>
@@ -2365,30 +2373,30 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Матылицкая Елена Юрьевна</t>
+          <t>Обучение 2</t>
         </is>
       </c>
       <c r="B19" s="18" t="n">
-        <v>32</v>
-      </c>
-      <c r="C19" s="22" t="inlineStr">
-        <is>
-          <t>270</t>
+        <v>49</v>
+      </c>
+      <c r="C19" s="23" t="inlineStr">
+        <is>
+          <t>352</t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>2:57:23</t>
+          <t>5:22:50</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>2:25:17</t>
+          <t>4:48:58</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>13:50</t>
+          <t>55:56</t>
         </is>
       </c>
       <c r="G19" s="3" t="inlineStr">
@@ -2398,7 +2406,7 @@
       </c>
       <c r="H19" s="3" t="inlineStr">
         <is>
-          <t>5:14</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I19" s="3" t="inlineStr">
@@ -2411,13 +2419,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K19" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L19" s="13" t="n">
-        <v>4</v>
+      <c r="K19" s="21" t="inlineStr">
+        <is>
+          <t>4.50</t>
+        </is>
+      </c>
+      <c r="L19" s="19" t="n">
+        <v>0</v>
       </c>
       <c r="M19" s="15" t="n"/>
       <c r="P19" s="15" t="n"/>
@@ -2426,30 +2434,30 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Обучение 1</t>
+          <t>Обучение ICL</t>
         </is>
       </c>
       <c r="B20" s="18" t="n">
-        <v>53</v>
-      </c>
-      <c r="C20" s="23" t="inlineStr">
-        <is>
-          <t>384</t>
+        <v>9</v>
+      </c>
+      <c r="C20" s="22" t="inlineStr">
+        <is>
+          <t>316</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>7:43:46</t>
+          <t>1:39:42</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>5:46:44</t>
+          <t>48:29</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>4:55:32</t>
+          <t>55:54</t>
         </is>
       </c>
       <c r="G20" s="3" t="inlineStr">
@@ -2459,12 +2467,12 @@
       </c>
       <c r="H20" s="3" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>3:35</t>
         </is>
       </c>
       <c r="I20" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>8:33</t>
         </is>
       </c>
       <c r="J20" s="3" t="inlineStr">
@@ -2472,13 +2480,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K20" s="21" t="inlineStr">
-        <is>
-          <t>4.75</t>
-        </is>
-      </c>
-      <c r="L20" s="10" t="n">
-        <v>0</v>
+      <c r="K20" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L20" s="21" t="n">
+        <v>4</v>
       </c>
       <c r="M20" s="15" t="n"/>
       <c r="P20" s="15" t="n"/>
@@ -2487,30 +2495,30 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Обучение 2</t>
+          <t>Орищенко Юлия Геннадьевна</t>
         </is>
       </c>
       <c r="B21" s="18" t="n">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C21" s="22" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>242</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>1:50:42</t>
+          <t>5:01:02</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>1:40:44</t>
+          <t>2:55:09</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>4:42:03</t>
+          <t>5:06</t>
         </is>
       </c>
       <c r="G21" s="3" t="inlineStr">
@@ -2533,13 +2541,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K21" s="21" t="inlineStr">
-        <is>
-          <t>4.00</t>
-        </is>
-      </c>
-      <c r="L21" s="10" t="n">
-        <v>0</v>
+      <c r="K21" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L21" s="23" t="n">
+        <v>50</v>
       </c>
       <c r="M21" s="15" t="n"/>
       <c r="P21" s="15" t="n"/>
@@ -2548,30 +2556,30 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>Обучение 3</t>
+          <t>Павликов Илья Сергеевич</t>
         </is>
       </c>
       <c r="B22" s="18" t="n">
-        <v>17</v>
-      </c>
-      <c r="C22" s="23" t="inlineStr">
-        <is>
-          <t>499</t>
+        <v>7</v>
+      </c>
+      <c r="C22" s="19" t="inlineStr">
+        <is>
+          <t>195</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
         <is>
-          <t>2:06:57</t>
+          <t>8:50:43</t>
         </is>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>2:25:46</t>
+          <t>23:17</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>2:52:18</t>
+          <t>7:00</t>
         </is>
       </c>
       <c r="G22" s="3" t="inlineStr">
@@ -2581,12 +2589,12 @@
       </c>
       <c r="H22" s="3" t="inlineStr">
         <is>
-          <t>41:53</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I22" s="3" t="inlineStr">
         <is>
-          <t>0:01</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J22" s="3" t="inlineStr">
@@ -2594,12 +2602,12 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K22" s="21" t="inlineStr">
-        <is>
-          <t>4.37</t>
-        </is>
-      </c>
-      <c r="L22" s="10" t="n">
+      <c r="K22" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L22" s="19" t="n">
         <v>0</v>
       </c>
       <c r="M22" s="15" t="n"/>
@@ -2609,45 +2617,45 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Обучение ICL</t>
+          <t>Плетнёв Владислав Евгеньевич</t>
         </is>
       </c>
       <c r="B23" s="18" t="n">
-        <v>54</v>
-      </c>
-      <c r="C23" s="23" t="inlineStr">
-        <is>
-          <t>450</t>
+        <v>30</v>
+      </c>
+      <c r="C23" s="19" t="inlineStr">
+        <is>
+          <t>168</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
-          <t>7:15:33</t>
+          <t>8:09:08</t>
         </is>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>6:47:54</t>
+          <t>1:27:26</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>31:55</t>
+          <t>4:01</t>
         </is>
       </c>
       <c r="G23" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>29:37</t>
         </is>
       </c>
       <c r="H23" s="3" t="inlineStr">
         <is>
-          <t>7:39</t>
+          <t>18:36</t>
         </is>
       </c>
       <c r="I23" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>14:36</t>
         </is>
       </c>
       <c r="J23" s="3" t="inlineStr">
@@ -2660,8 +2668,8 @@
           <t>5.00</t>
         </is>
       </c>
-      <c r="L23" s="10" t="n">
-        <v>0</v>
+      <c r="L23" s="21" t="n">
+        <v>4</v>
       </c>
       <c r="M23" s="15" t="n"/>
       <c r="P23" s="15" t="n"/>
@@ -2674,26 +2682,26 @@
         </is>
       </c>
       <c r="B24" s="18" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C24" s="23" t="inlineStr">
         <is>
-          <t>486</t>
+          <t>379</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
         <is>
-          <t>2:47:29</t>
+          <t>3:03:06</t>
         </is>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>1:57:46</t>
+          <t>1:16:50</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>1:03:02</t>
+          <t>4:27:04</t>
         </is>
       </c>
       <c r="G24" s="3" t="inlineStr">
@@ -2716,12 +2724,12 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K24" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L24" s="10" t="n">
+      <c r="K24" s="21" t="inlineStr">
+        <is>
+          <t>4.33</t>
+        </is>
+      </c>
+      <c r="L24" s="19" t="n">
         <v>0</v>
       </c>
       <c r="M24" s="15" t="n"/>
@@ -2735,26 +2743,26 @@
         </is>
       </c>
       <c r="B25" s="18" t="n">
-        <v>33</v>
-      </c>
-      <c r="C25" s="21" t="inlineStr">
-        <is>
-          <t>238</t>
+        <v>22</v>
+      </c>
+      <c r="C25" s="23" t="inlineStr">
+        <is>
+          <t>355</t>
         </is>
       </c>
       <c r="D25" s="3" t="inlineStr">
         <is>
-          <t>3:07:17</t>
+          <t>3:06:14</t>
         </is>
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>2:12:38</t>
+          <t>2:11:24</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>27:05</t>
+          <t>43:45</t>
         </is>
       </c>
       <c r="G25" s="3" t="inlineStr">
@@ -2764,7 +2772,7 @@
       </c>
       <c r="H25" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>1:37</t>
         </is>
       </c>
       <c r="I25" s="3" t="inlineStr">
@@ -2782,8 +2790,8 @@
           <t>5.00</t>
         </is>
       </c>
-      <c r="L25" s="14" t="n">
-        <v>1</v>
+      <c r="L25" s="19" t="n">
+        <v>0</v>
       </c>
       <c r="M25" s="15" t="n"/>
       <c r="P25" s="15" t="n"/>
@@ -2792,30 +2800,30 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>Севостьянов Михаил Игоревич</t>
-        </is>
-      </c>
-      <c r="B26" s="18" t="n">
-        <v>10</v>
-      </c>
-      <c r="C26" s="21" t="inlineStr">
-        <is>
-          <t>235</t>
+          <t>Серова Юлия Владимировна</t>
+        </is>
+      </c>
+      <c r="B26" s="19" t="n">
+        <v>61</v>
+      </c>
+      <c r="C26" s="22" t="inlineStr">
+        <is>
+          <t>300</t>
         </is>
       </c>
       <c r="D26" s="3" t="inlineStr">
         <is>
-          <t>1:38:55</t>
+          <t>7:08:30</t>
         </is>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>40:01</t>
+          <t>5:13:38</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>2:12</t>
+          <t>2:44:13</t>
         </is>
       </c>
       <c r="G26" s="3" t="inlineStr">
@@ -2825,7 +2833,7 @@
       </c>
       <c r="H26" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>7:13</t>
         </is>
       </c>
       <c r="I26" s="3" t="inlineStr">
@@ -2838,13 +2846,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K26" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L26" s="13" t="n">
-        <v>3</v>
+      <c r="K26" s="21" t="inlineStr">
+        <is>
+          <t>4.60</t>
+        </is>
+      </c>
+      <c r="L26" s="23" t="n">
+        <v>26</v>
       </c>
       <c r="M26" s="15" t="n"/>
       <c r="P26" s="15" t="n"/>
@@ -2853,30 +2861,30 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>Серова Юлия Владимировна</t>
+          <t>Силин Егор Владимирович</t>
         </is>
       </c>
       <c r="B27" s="18" t="n">
-        <v>51</v>
-      </c>
-      <c r="C27" s="21" t="inlineStr">
-        <is>
-          <t>237</t>
+        <v>44</v>
+      </c>
+      <c r="C27" s="23" t="inlineStr">
+        <is>
+          <t>343</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
         <is>
-          <t>3:50:30</t>
+          <t>5:33:40</t>
         </is>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>3:27:24</t>
+          <t>4:15:19</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>5:55</t>
+          <t>1:00:05</t>
         </is>
       </c>
       <c r="G27" s="3" t="inlineStr">
@@ -2886,7 +2894,7 @@
       </c>
       <c r="H27" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>22:36</t>
         </is>
       </c>
       <c r="I27" s="3" t="inlineStr">
@@ -2896,16 +2904,16 @@
       </c>
       <c r="J27" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
-        </is>
-      </c>
-      <c r="K27" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L27" s="13" t="n">
-        <v>4</v>
+          <t>0:01</t>
+        </is>
+      </c>
+      <c r="K27" s="21" t="inlineStr">
+        <is>
+          <t>4.84</t>
+        </is>
+      </c>
+      <c r="L27" s="21" t="n">
+        <v>3</v>
       </c>
       <c r="M27" s="15" t="n"/>
       <c r="P27" s="15" t="n"/>
@@ -2914,30 +2922,30 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>Стаценко Юлия Валентиновна</t>
+          <t>Смертина София Сергеевна</t>
         </is>
       </c>
       <c r="B28" s="18" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C28" s="22" t="inlineStr">
         <is>
-          <t>331</t>
+          <t>265</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
         <is>
-          <t>1:59:40</t>
+          <t>1:59:48</t>
         </is>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>1:06:56</t>
+          <t>1:07:55</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t>8:18</t>
+          <t>9:17</t>
         </is>
       </c>
       <c r="G28" s="3" t="inlineStr">
@@ -2965,8 +2973,8 @@
           <t>5.00</t>
         </is>
       </c>
-      <c r="L28" s="13" t="n">
-        <v>5</v>
+      <c r="L28" s="24" t="n">
+        <v>1</v>
       </c>
       <c r="M28" s="15" t="n"/>
       <c r="P28" s="15" t="n"/>
@@ -2979,26 +2987,26 @@
         </is>
       </c>
       <c r="B29" s="18" t="n">
-        <v>24</v>
-      </c>
-      <c r="C29" s="22" t="inlineStr">
-        <is>
-          <t>291</t>
+        <v>49</v>
+      </c>
+      <c r="C29" s="19" t="inlineStr">
+        <is>
+          <t>158</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
-          <t>2:57:37</t>
+          <t>2:50:01</t>
         </is>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>1:59:29</t>
+          <t>2:14:23</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>45:42</t>
+          <t>22:01</t>
         </is>
       </c>
       <c r="G29" s="3" t="inlineStr">
@@ -3008,7 +3016,7 @@
       </c>
       <c r="H29" s="3" t="inlineStr">
         <is>
-          <t>10:02</t>
+          <t>8:39</t>
         </is>
       </c>
       <c r="I29" s="3" t="inlineStr">
@@ -3021,12 +3029,12 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K29" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L29" s="13" t="n">
+      <c r="K29" s="22" t="inlineStr">
+        <is>
+          <t>3.80</t>
+        </is>
+      </c>
+      <c r="L29" s="21" t="n">
         <v>5</v>
       </c>
       <c r="M29" s="15" t="n"/>
@@ -3036,30 +3044,30 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>Шартнер Елена Александровна</t>
+          <t>Шамли Алина Алексеевна</t>
         </is>
       </c>
       <c r="B30" s="18" t="n">
-        <v>46</v>
-      </c>
-      <c r="C30" s="19" t="inlineStr">
-        <is>
-          <t>189</t>
+        <v>9</v>
+      </c>
+      <c r="C30" s="23" t="inlineStr">
+        <is>
+          <t>590</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
         <is>
-          <t>3:01:03</t>
+          <t>1:45:13</t>
         </is>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>2:28:24</t>
+          <t>1:29:07</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
         <is>
-          <t>23:51</t>
+          <t>31:53</t>
         </is>
       </c>
       <c r="G30" s="3" t="inlineStr">
@@ -3084,38 +3092,40 @@
       </c>
       <c r="K30" s="21" t="inlineStr">
         <is>
-          <t>4.50</t>
-        </is>
-      </c>
-      <c r="L30" s="13" t="n"/>
+          <t>4.20</t>
+        </is>
+      </c>
+      <c r="L30" s="19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>Яценко Александра Андреевна</t>
+          <t>Шартнер Елена Александровна</t>
         </is>
       </c>
       <c r="B31" s="18" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C31" s="21" t="inlineStr">
         <is>
-          <t>202</t>
+          <t>232</t>
         </is>
       </c>
       <c r="D31" s="3" t="inlineStr">
         <is>
-          <t>1:58:20</t>
+          <t>3:42:38</t>
         </is>
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>34:51</t>
+          <t>1:55:47</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>29:02</t>
+          <t>4:28</t>
         </is>
       </c>
       <c r="G31" s="3" t="inlineStr">
@@ -3130,7 +3140,7 @@
       </c>
       <c r="I31" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="J31" s="3" t="inlineStr">
@@ -3143,21 +3153,67 @@
           <t>5.00</t>
         </is>
       </c>
-      <c r="L31" s="13" t="n"/>
+      <c r="L31" s="21" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="n"/>
-      <c r="B32" s="3" t="n"/>
-      <c r="C32" s="10" t="n"/>
-      <c r="D32" s="3" t="n"/>
-      <c r="E32" s="3" t="n"/>
-      <c r="F32" s="3" t="n"/>
-      <c r="G32" s="3" t="n"/>
-      <c r="H32" s="3" t="n"/>
-      <c r="I32" s="3" t="n"/>
-      <c r="J32" s="3" t="n"/>
-      <c r="K32" s="10" t="n"/>
-      <c r="L32" s="13" t="n"/>
+      <c r="A32" s="3" t="inlineStr">
+        <is>
+          <t>Шептунова Софья Денисовна</t>
+        </is>
+      </c>
+      <c r="B32" s="18" t="n">
+        <v>31</v>
+      </c>
+      <c r="C32" s="22" t="inlineStr">
+        <is>
+          <t>249</t>
+        </is>
+      </c>
+      <c r="D32" s="3" t="inlineStr">
+        <is>
+          <t>3:04:12</t>
+        </is>
+      </c>
+      <c r="E32" s="3" t="inlineStr">
+        <is>
+          <t>2:10:37</t>
+        </is>
+      </c>
+      <c r="F32" s="3" t="inlineStr">
+        <is>
+          <t>1:04</t>
+        </is>
+      </c>
+      <c r="G32" s="3" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="K32" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L32" s="21" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="n"/>

</xml_diff>

<commit_message>
work 1.2.0 week report
</commit_message>
<xml_diff>
--- a/files_samples/Статистика операторов с пропущенными.xlsx
+++ b/files_samples/Статистика операторов с пропущенными.xlsx
@@ -1318,7 +1318,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Среда, 13.11.2024</t>
+          <t>Четверг, 14.11.2024</t>
         </is>
       </c>
       <c r="B1" s="16" t="n"/>
@@ -1402,26 +1402,26 @@
         </is>
       </c>
       <c r="B3" s="18" t="n">
-        <v>9</v>
-      </c>
-      <c r="C3" s="22" t="inlineStr">
-        <is>
-          <t>294</t>
+        <v>27</v>
+      </c>
+      <c r="C3" s="20" t="inlineStr">
+        <is>
+          <t>109</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>1:55:13</t>
+          <t>7:34:00</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>44:41</t>
+          <t>57:42</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>3:42</t>
+          <t>57:52</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="I3" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>5:43</t>
         </is>
       </c>
       <c r="J3" s="3" t="inlineStr">
@@ -1444,13 +1444,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K3" s="21" t="inlineStr">
-        <is>
-          <t>4.83</t>
+      <c r="K3" s="22" t="inlineStr">
+        <is>
+          <t>4.85</t>
         </is>
       </c>
       <c r="L3" s="19" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="M3" s="15" t="n"/>
       <c r="P3" s="15" t="n"/>
@@ -1463,41 +1463,41 @@
         </is>
       </c>
       <c r="B4" s="19" t="n">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C4" s="19" t="inlineStr">
         <is>
-          <t>189</t>
+          <t>179</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>6:43:58</t>
+          <t>7:03:20</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>3:38:10</t>
+          <t>4:09:22</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>34:35</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">
         <is>
-          <t>29:15</t>
+          <t>30:05</t>
         </is>
       </c>
       <c r="H4" s="3" t="inlineStr">
         <is>
-          <t>10:08</t>
+          <t>10:10</t>
         </is>
       </c>
       <c r="I4" s="3" t="inlineStr">
         <is>
-          <t>23:09</t>
+          <t>1:46</t>
         </is>
       </c>
       <c r="J4" s="3" t="inlineStr">
@@ -1505,13 +1505,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K4" s="21" t="inlineStr">
-        <is>
-          <t>4.80</t>
-        </is>
-      </c>
-      <c r="L4" s="19" t="n">
-        <v>0</v>
+      <c r="K4" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L4" s="24" t="n">
+        <v>1</v>
       </c>
       <c r="M4" s="15" t="n"/>
       <c r="P4" s="15" t="n"/>
@@ -1524,26 +1524,26 @@
         </is>
       </c>
       <c r="B5" s="18" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C5" s="23" t="inlineStr">
         <is>
-          <t>437</t>
+          <t>528</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>5:57:56</t>
+          <t>1:08:40</t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>1:58:28</t>
+          <t>9:18</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>0:56</t>
+          <t>11:29</t>
         </is>
       </c>
       <c r="G5" s="3" t="inlineStr">
@@ -1558,7 +1558,7 @@
       </c>
       <c r="I5" s="3" t="inlineStr">
         <is>
-          <t>8:44</t>
+          <t>3:12</t>
         </is>
       </c>
       <c r="J5" s="3" t="inlineStr">
@@ -1566,13 +1566,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K5" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
+      <c r="K5" s="22" t="inlineStr">
+        <is>
+          <t>0.00</t>
         </is>
       </c>
       <c r="L5" s="21" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M5" s="15" t="n"/>
       <c r="P5" s="15" t="n"/>
@@ -1581,59 +1581,59 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Горных Ксения Сергеевна</t>
-        </is>
-      </c>
-      <c r="B6" s="18" t="n">
-        <v>55</v>
-      </c>
-      <c r="C6" s="21" t="inlineStr">
-        <is>
-          <t>231</t>
+          <t>Гарипова Лейсан Миневелиевна</t>
+        </is>
+      </c>
+      <c r="B6" s="19" t="n">
+        <v>77</v>
+      </c>
+      <c r="C6" s="22" t="inlineStr">
+        <is>
+          <t>297</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>4:59:08</t>
+          <t>9:18:53</t>
         </is>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>3:36:47</t>
+          <t>6:25:53</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>1:31</t>
+          <t>1:38</t>
         </is>
       </c>
       <c r="G6" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>28:23</t>
         </is>
       </c>
       <c r="H6" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>11:34</t>
         </is>
       </c>
       <c r="I6" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>2:57</t>
         </is>
       </c>
       <c r="J6" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>48:09</t>
         </is>
       </c>
       <c r="K6" s="21" t="inlineStr">
         <is>
-          <t>4.68</t>
+          <t>4.97</t>
         </is>
       </c>
       <c r="L6" s="21" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M6" s="15" t="n"/>
       <c r="P6" s="15" t="n"/>
@@ -1642,30 +1642,30 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Гребенюк Полина Максимовна</t>
+          <t>Гарифуллин Булат Дамирович</t>
         </is>
       </c>
       <c r="B7" s="18" t="n">
-        <v>25</v>
-      </c>
-      <c r="C7" s="21" t="inlineStr">
-        <is>
-          <t>224</t>
+        <v>21</v>
+      </c>
+      <c r="C7" s="19" t="inlineStr">
+        <is>
+          <t>186</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>2:16:19</t>
+          <t>2:24:51</t>
         </is>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>1:33:57</t>
+          <t>1:07:38</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>4:25</t>
+          <t>42:15</t>
         </is>
       </c>
       <c r="G7" s="3" t="inlineStr">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="H7" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>7:00</t>
         </is>
       </c>
       <c r="I7" s="3" t="inlineStr">
@@ -1688,13 +1688,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K7" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L7" s="19" t="n">
-        <v>0</v>
+      <c r="K7" s="21" t="inlineStr">
+        <is>
+          <t>4.50</t>
+        </is>
+      </c>
+      <c r="L7" s="24" t="n">
+        <v>1</v>
       </c>
       <c r="M7" s="15" t="n"/>
       <c r="P7" s="15" t="n"/>
@@ -1703,35 +1703,35 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>Джабраилова Елена Валерьевна</t>
-        </is>
-      </c>
-      <c r="B8" s="20" t="n">
-        <v>148</v>
-      </c>
-      <c r="C8" s="19" t="inlineStr">
-        <is>
-          <t>180</t>
+          <t>Горных Ксения Сергеевна</t>
+        </is>
+      </c>
+      <c r="B8" s="18" t="n">
+        <v>64</v>
+      </c>
+      <c r="C8" s="21" t="inlineStr">
+        <is>
+          <t>226</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>10:47:49</t>
+          <t>6:58:14</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>7:36:25</t>
+          <t>4:06:05</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>2:33</t>
+          <t>1:39:47</t>
         </is>
       </c>
       <c r="G8" s="3" t="inlineStr">
         <is>
-          <t>30:03</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="H8" s="3" t="inlineStr">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="I8" s="3" t="inlineStr">
         <is>
-          <t>29:18</t>
+          <t>3:22</t>
         </is>
       </c>
       <c r="J8" s="3" t="inlineStr">
@@ -1749,13 +1749,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K8" s="22" t="inlineStr">
-        <is>
-          <t>4.70</t>
-        </is>
-      </c>
-      <c r="L8" s="13" t="n">
-        <v>11</v>
+      <c r="K8" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L8" s="21" t="n">
+        <v>6</v>
       </c>
       <c r="M8" s="15" t="n"/>
       <c r="P8" s="15" t="n"/>
@@ -1764,30 +1764,30 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>Довыдович Алиса Станиславовна</t>
+          <t>Гребенюк Полина Максимовна</t>
         </is>
       </c>
       <c r="B9" s="18" t="n">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C9" s="19" t="inlineStr">
         <is>
-          <t>177</t>
+          <t>178</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>1:59:50</t>
+          <t>5:48:35</t>
         </is>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>1:34:54</t>
+          <t>2:45:11</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>13:40</t>
+          <t>2:31</t>
         </is>
       </c>
       <c r="G9" s="3" t="inlineStr">
@@ -1797,12 +1797,12 @@
       </c>
       <c r="H9" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>11:24</t>
         </is>
       </c>
       <c r="I9" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>2:13</t>
         </is>
       </c>
       <c r="J9" s="3" t="inlineStr">
@@ -1810,13 +1810,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K9" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L9" s="19" t="n">
-        <v>0</v>
+      <c r="K9" s="21" t="inlineStr">
+        <is>
+          <t>4.80</t>
+        </is>
+      </c>
+      <c r="L9" s="24" t="n">
+        <v>1</v>
       </c>
       <c r="M9" s="15" t="n"/>
       <c r="Q9" s="15" t="n"/>
@@ -1824,35 +1824,35 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>Егоров Олег Александрович</t>
-        </is>
-      </c>
-      <c r="B10" s="18" t="n">
-        <v>45</v>
-      </c>
-      <c r="C10" s="20" t="inlineStr">
-        <is>
-          <t>140</t>
+          <t>Джабраилова Елена Валерьевна</t>
+        </is>
+      </c>
+      <c r="B10" s="20" t="n">
+        <v>142</v>
+      </c>
+      <c r="C10" s="19" t="inlineStr">
+        <is>
+          <t>185</t>
         </is>
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>1:44:38</t>
+          <t>11:25:05</t>
         </is>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>1:45:22</t>
+          <t>7:29:17</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>10:19:38</t>
+          <t>1:09</t>
         </is>
       </c>
       <c r="G10" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>33:54</t>
         </is>
       </c>
       <c r="H10" s="3" t="inlineStr">
@@ -1862,7 +1862,7 @@
       </c>
       <c r="I10" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>2:05</t>
         </is>
       </c>
       <c r="J10" s="3" t="inlineStr">
@@ -1870,13 +1870,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K10" s="21" t="inlineStr">
-        <is>
-          <t>4.89</t>
+      <c r="K10" s="22" t="inlineStr">
+        <is>
+          <t>4.78</t>
         </is>
       </c>
       <c r="L10" s="21" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="M10" s="15" t="n"/>
       <c r="P10" s="15" t="n"/>
@@ -1885,40 +1885,40 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Жданов Денис Александрович</t>
+          <t>Довыдович Алиса Станиславовна</t>
         </is>
       </c>
       <c r="B11" s="18" t="n">
-        <v>56</v>
-      </c>
-      <c r="C11" s="22" t="inlineStr">
-        <is>
-          <t>268</t>
+        <v>57</v>
+      </c>
+      <c r="C11" s="21" t="inlineStr">
+        <is>
+          <t>231</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>4:43:23</t>
+          <t>5:40:38</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>4:13:22</t>
+          <t>3:40:53</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>5:07</t>
+          <t>16:03</t>
         </is>
       </c>
       <c r="G11" s="3" t="inlineStr">
         <is>
-          <t>0:08</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="H11" s="3" t="inlineStr">
         <is>
-          <t>4:51</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I11" s="3" t="inlineStr">
@@ -1928,12 +1928,12 @@
       </c>
       <c r="J11" s="3" t="inlineStr">
         <is>
-          <t>16:13</t>
-        </is>
-      </c>
-      <c r="K11" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="K11" s="21" t="inlineStr">
+        <is>
+          <t>4.55</t>
         </is>
       </c>
       <c r="L11" s="19" t="n">
@@ -1946,30 +1946,30 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>Жевнер Григорий Павлович</t>
+          <t>Егоров Олег Александрович</t>
         </is>
       </c>
       <c r="B12" s="18" t="n">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="C12" s="20" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>115</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>3:03:56</t>
+          <t>1:34:51</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>32:03</t>
+          <t>1:37:12</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>46:28</t>
+          <t>10:28:54</t>
         </is>
       </c>
       <c r="G12" s="3" t="inlineStr">
@@ -1992,13 +1992,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K12" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L12" s="19" t="n">
-        <v>0</v>
+      <c r="K12" s="21" t="inlineStr">
+        <is>
+          <t>4.72</t>
+        </is>
+      </c>
+      <c r="L12" s="24" t="n">
+        <v>1</v>
       </c>
       <c r="M12" s="15" t="n"/>
       <c r="P12" s="15" t="n"/>
@@ -2007,35 +2007,35 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Зиберт Ольга Николаевна</t>
+          <t>Жевнер Григорий Павлович</t>
         </is>
       </c>
       <c r="B13" s="18" t="n">
-        <v>24</v>
-      </c>
-      <c r="C13" s="23" t="inlineStr">
-        <is>
-          <t>434</t>
+        <v>8</v>
+      </c>
+      <c r="C13" s="20" t="inlineStr">
+        <is>
+          <t>99</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>3:25:13</t>
+          <t>8:36:51</t>
         </is>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>2:55:45</t>
+          <t>14:48</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>29:57</t>
+          <t>11:08</t>
         </is>
       </c>
       <c r="G13" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>8:46</t>
         </is>
       </c>
       <c r="H13" s="3" t="inlineStr">
@@ -2053,13 +2053,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K13" s="21" t="inlineStr">
-        <is>
-          <t>4.33</t>
-        </is>
-      </c>
-      <c r="L13" s="21" t="n">
-        <v>2</v>
+      <c r="K13" s="22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L13" s="19" t="n">
+        <v>0</v>
       </c>
       <c r="M13" s="15" t="n"/>
       <c r="P13" s="15" t="n"/>
@@ -2068,30 +2068,30 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>Клочкова София Антоновна</t>
+          <t>Зиберт Ольга Николаевна</t>
         </is>
       </c>
       <c r="B14" s="18" t="n">
-        <v>22</v>
-      </c>
-      <c r="C14" s="22" t="inlineStr">
-        <is>
-          <t>295</t>
+        <v>23</v>
+      </c>
+      <c r="C14" s="23" t="inlineStr">
+        <is>
+          <t>499</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>2:08:15</t>
+          <t>3:58:16</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>1:49:05</t>
+          <t>3:12:44</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>42:42</t>
+          <t>24:55</t>
         </is>
       </c>
       <c r="G14" s="3" t="inlineStr">
@@ -2106,7 +2106,7 @@
       </c>
       <c r="I14" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>1:41</t>
         </is>
       </c>
       <c r="J14" s="3" t="inlineStr">
@@ -2114,13 +2114,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K14" s="22" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="L14" s="19" t="n">
-        <v>0</v>
+      <c r="K14" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L14" s="24" t="n">
+        <v>1</v>
       </c>
       <c r="M14" s="15" t="n"/>
       <c r="P14" s="15" t="n"/>
@@ -2129,30 +2129,30 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>Маркелов Сергей Алексеевич</t>
+          <t>Куликов Максим Геннадьевич</t>
         </is>
       </c>
       <c r="B15" s="18" t="n">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C15" s="19" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>150</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>9:49:39</t>
+          <t>2:38:26</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>2:35:50</t>
+          <t>31:09</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>52:01</t>
+          <t>0:14</t>
         </is>
       </c>
       <c r="G15" s="3" t="inlineStr">
@@ -2162,26 +2162,26 @@
       </c>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>9:48</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I15" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>4:29</t>
         </is>
       </c>
       <c r="J15" s="3" t="inlineStr">
         <is>
-          <t>1:58:54</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="K15" s="21" t="inlineStr">
         <is>
-          <t>4.61</t>
-        </is>
-      </c>
-      <c r="L15" s="21" t="n">
-        <v>2</v>
+          <t>4.60</t>
+        </is>
+      </c>
+      <c r="L15" s="24" t="n">
+        <v>1</v>
       </c>
       <c r="M15" s="15" t="n"/>
       <c r="P15" s="15" t="n"/>
@@ -2194,26 +2194,26 @@
         </is>
       </c>
       <c r="B16" s="18" t="n">
-        <v>26</v>
-      </c>
-      <c r="C16" s="22" t="inlineStr">
-        <is>
-          <t>285</t>
+        <v>13</v>
+      </c>
+      <c r="C16" s="23" t="inlineStr">
+        <is>
+          <t>520</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>2:58:13</t>
+          <t>1:59:44</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>2:05:25</t>
+          <t>1:53:04</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>34:05</t>
+          <t>3:09</t>
         </is>
       </c>
       <c r="G16" s="3" t="inlineStr">
@@ -2223,7 +2223,7 @@
       </c>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>7:32</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I16" s="3" t="inlineStr">
@@ -2236,9 +2236,9 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K16" s="21" t="inlineStr">
-        <is>
-          <t>4.92</t>
+      <c r="K16" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
         </is>
       </c>
       <c r="L16" s="19" t="n">
@@ -2255,26 +2255,26 @@
         </is>
       </c>
       <c r="B17" s="18" t="n">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C17" s="19" t="inlineStr">
         <is>
-          <t>191</t>
+          <t>200</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>4:01:17</t>
+          <t>3:53:58</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>2:20:59</t>
+          <t>3:06:54</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>6:01</t>
+          <t>30:30</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
@@ -2297,13 +2297,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K17" s="22" t="inlineStr">
-        <is>
-          <t>4.46</t>
-        </is>
-      </c>
-      <c r="L17" s="11" t="n">
-        <v>12</v>
+      <c r="K17" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L17" s="21" t="n">
+        <v>7</v>
       </c>
       <c r="M17" s="15" t="n"/>
       <c r="P17" s="15" t="n"/>
@@ -2316,26 +2316,26 @@
         </is>
       </c>
       <c r="B18" s="18" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C18" s="23" t="inlineStr">
         <is>
-          <t>616</t>
+          <t>558</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>2:06:24</t>
+          <t>1:59:52</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>1:43:26</t>
+          <t>1:53:04</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>1.06:54:14</t>
+          <t>12:47:11</t>
         </is>
       </c>
       <c r="G18" s="3" t="inlineStr">
@@ -2373,30 +2373,30 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Обучение 2</t>
+          <t>Орищенко Юлия Геннадьевна</t>
         </is>
       </c>
       <c r="B19" s="18" t="n">
-        <v>49</v>
-      </c>
-      <c r="C19" s="23" t="inlineStr">
-        <is>
-          <t>352</t>
+        <v>37</v>
+      </c>
+      <c r="C19" s="21" t="inlineStr">
+        <is>
+          <t>216</t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>5:22:50</t>
+          <t>4:37:24</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>4:48:58</t>
+          <t>2:21:16</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>55:56</t>
+          <t>2:58</t>
         </is>
       </c>
       <c r="G19" s="3" t="inlineStr">
@@ -2411,7 +2411,7 @@
       </c>
       <c r="I19" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>1:36</t>
         </is>
       </c>
       <c r="J19" s="3" t="inlineStr">
@@ -2421,11 +2421,11 @@
       </c>
       <c r="K19" s="21" t="inlineStr">
         <is>
-          <t>4.50</t>
-        </is>
-      </c>
-      <c r="L19" s="19" t="n">
-        <v>0</v>
+          <t>4.42</t>
+        </is>
+      </c>
+      <c r="L19" s="23" t="n">
+        <v>33</v>
       </c>
       <c r="M19" s="15" t="n"/>
       <c r="P19" s="15" t="n"/>
@@ -2434,30 +2434,30 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Обучение ICL</t>
+          <t>Павликов Илья Сергеевич</t>
         </is>
       </c>
       <c r="B20" s="18" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C20" s="22" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>315</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>1:39:42</t>
+          <t>2:24:00</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>48:29</t>
+          <t>13:36</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>55:54</t>
+          <t>14:27</t>
         </is>
       </c>
       <c r="G20" s="3" t="inlineStr">
@@ -2467,12 +2467,12 @@
       </c>
       <c r="H20" s="3" t="inlineStr">
         <is>
-          <t>3:35</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I20" s="3" t="inlineStr">
         <is>
-          <t>8:33</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J20" s="3" t="inlineStr">
@@ -2485,8 +2485,8 @@
           <t>5.00</t>
         </is>
       </c>
-      <c r="L20" s="21" t="n">
-        <v>4</v>
+      <c r="L20" s="19" t="n">
+        <v>0</v>
       </c>
       <c r="M20" s="15" t="n"/>
       <c r="P20" s="15" t="n"/>
@@ -2495,30 +2495,30 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Орищенко Юлия Геннадьевна</t>
+          <t>Плетнёв Владислав Евгеньевич</t>
         </is>
       </c>
       <c r="B21" s="18" t="n">
-        <v>41</v>
-      </c>
-      <c r="C21" s="22" t="inlineStr">
-        <is>
-          <t>242</t>
+        <v>36</v>
+      </c>
+      <c r="C21" s="21" t="inlineStr">
+        <is>
+          <t>208</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>5:01:02</t>
+          <t>7:38:29</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>2:55:09</t>
+          <t>2:09:29</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>5:06</t>
+          <t>0:56</t>
         </is>
       </c>
       <c r="G21" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
       </c>
       <c r="H21" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>27:17</t>
         </is>
       </c>
       <c r="I21" s="3" t="inlineStr">
@@ -2541,13 +2541,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K21" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L21" s="23" t="n">
-        <v>50</v>
+      <c r="K21" s="21" t="inlineStr">
+        <is>
+          <t>4.93</t>
+        </is>
+      </c>
+      <c r="L21" s="21" t="n">
+        <v>6</v>
       </c>
       <c r="M21" s="15" t="n"/>
       <c r="P21" s="15" t="n"/>
@@ -2556,30 +2556,30 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>Павликов Илья Сергеевич</t>
+          <t>Путко Екатерина Николаевна</t>
         </is>
       </c>
       <c r="B22" s="18" t="n">
-        <v>7</v>
-      </c>
-      <c r="C22" s="19" t="inlineStr">
-        <is>
-          <t>195</t>
+        <v>10</v>
+      </c>
+      <c r="C22" s="23" t="inlineStr">
+        <is>
+          <t>353</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
         <is>
-          <t>8:50:43</t>
+          <t>2:47:10</t>
         </is>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>23:17</t>
+          <t>59:58</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>7:00</t>
+          <t>2:13:39</t>
         </is>
       </c>
       <c r="G22" s="3" t="inlineStr">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="I22" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>8:36</t>
         </is>
       </c>
       <c r="J22" s="3" t="inlineStr">
@@ -2607,8 +2607,8 @@
           <t>5.00</t>
         </is>
       </c>
-      <c r="L22" s="19" t="n">
-        <v>0</v>
+      <c r="L22" s="21" t="n">
+        <v>2</v>
       </c>
       <c r="M22" s="15" t="n"/>
       <c r="P22" s="15" t="n"/>
@@ -2617,45 +2617,45 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Плетнёв Владислав Евгеньевич</t>
+          <t>Рыжкина Екатерина Михайловна</t>
         </is>
       </c>
       <c r="B23" s="18" t="n">
-        <v>30</v>
-      </c>
-      <c r="C23" s="19" t="inlineStr">
-        <is>
-          <t>168</t>
+        <v>31</v>
+      </c>
+      <c r="C23" s="21" t="inlineStr">
+        <is>
+          <t>222</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
-          <t>8:09:08</t>
+          <t>3:02:42</t>
         </is>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>1:27:26</t>
+          <t>1:56:04</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>4:01</t>
+          <t>19:52</t>
         </is>
       </c>
       <c r="G23" s="3" t="inlineStr">
         <is>
-          <t>29:37</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="H23" s="3" t="inlineStr">
         <is>
-          <t>18:36</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I23" s="3" t="inlineStr">
         <is>
-          <t>14:36</t>
+          <t>2:04</t>
         </is>
       </c>
       <c r="J23" s="3" t="inlineStr">
@@ -2663,13 +2663,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K23" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L23" s="21" t="n">
-        <v>4</v>
+      <c r="K23" s="21" t="inlineStr">
+        <is>
+          <t>4.83</t>
+        </is>
+      </c>
+      <c r="L23" s="19" t="n">
+        <v>0</v>
       </c>
       <c r="M23" s="15" t="n"/>
       <c r="P23" s="15" t="n"/>
@@ -2678,30 +2678,30 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>Путко Екатерина Николаевна</t>
+          <t>Севостьянов Михаил Игоревич</t>
         </is>
       </c>
       <c r="B24" s="18" t="n">
-        <v>12</v>
-      </c>
-      <c r="C24" s="23" t="inlineStr">
-        <is>
-          <t>379</t>
+        <v>35</v>
+      </c>
+      <c r="C24" s="22" t="inlineStr">
+        <is>
+          <t>272</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
         <is>
-          <t>3:03:06</t>
+          <t>4:41:18</t>
         </is>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>1:16:50</t>
+          <t>2:43:16</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>4:27:04</t>
+          <t>2:40</t>
         </is>
       </c>
       <c r="G24" s="3" t="inlineStr">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="I24" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>4:51</t>
         </is>
       </c>
       <c r="J24" s="3" t="inlineStr">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="K24" s="21" t="inlineStr">
         <is>
-          <t>4.33</t>
+          <t>4.90</t>
         </is>
       </c>
       <c r="L24" s="19" t="n">
@@ -2739,30 +2739,30 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>Рыжкина Екатерина Михайловна</t>
+          <t>Серова Юлия Владимировна</t>
         </is>
       </c>
       <c r="B25" s="18" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C25" s="23" t="inlineStr">
         <is>
-          <t>355</t>
+          <t>356</t>
         </is>
       </c>
       <c r="D25" s="3" t="inlineStr">
         <is>
-          <t>3:06:14</t>
+          <t>3:40:01</t>
         </is>
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>2:11:24</t>
+          <t>3:01:16</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>43:45</t>
+          <t>6:06</t>
         </is>
       </c>
       <c r="G25" s="3" t="inlineStr">
@@ -2772,7 +2772,7 @@
       </c>
       <c r="H25" s="3" t="inlineStr">
         <is>
-          <t>1:37</t>
+          <t>9:18</t>
         </is>
       </c>
       <c r="I25" s="3" t="inlineStr">
@@ -2785,13 +2785,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K25" s="19" t="inlineStr">
+      <c r="K25" s="22" t="inlineStr">
         <is>
           <t>5.00</t>
         </is>
       </c>
       <c r="L25" s="19" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M25" s="15" t="n"/>
       <c r="P25" s="15" t="n"/>
@@ -2800,30 +2800,30 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>Серова Юлия Владимировна</t>
-        </is>
-      </c>
-      <c r="B26" s="19" t="n">
-        <v>61</v>
-      </c>
-      <c r="C26" s="22" t="inlineStr">
-        <is>
-          <t>300</t>
+          <t>Силин Егор Владимирович</t>
+        </is>
+      </c>
+      <c r="B26" s="18" t="n">
+        <v>27</v>
+      </c>
+      <c r="C26" s="23" t="inlineStr">
+        <is>
+          <t>365</t>
         </is>
       </c>
       <c r="D26" s="3" t="inlineStr">
         <is>
-          <t>7:08:30</t>
+          <t>4:11:28</t>
         </is>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>5:13:38</t>
+          <t>2:46:43</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>2:44:13</t>
+          <t>43:03</t>
         </is>
       </c>
       <c r="G26" s="3" t="inlineStr">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="H26" s="3" t="inlineStr">
         <is>
-          <t>7:13</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="I26" s="3" t="inlineStr">
@@ -2846,13 +2846,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K26" s="21" t="inlineStr">
-        <is>
-          <t>4.60</t>
-        </is>
-      </c>
-      <c r="L26" s="23" t="n">
-        <v>26</v>
+      <c r="K26" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L26" s="24" t="n">
+        <v>1</v>
       </c>
       <c r="M26" s="15" t="n"/>
       <c r="P26" s="15" t="n"/>
@@ -2861,30 +2861,30 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>Силин Егор Владимирович</t>
+          <t>Смертина София Сергеевна</t>
         </is>
       </c>
       <c r="B27" s="18" t="n">
-        <v>44</v>
-      </c>
-      <c r="C27" s="23" t="inlineStr">
-        <is>
-          <t>343</t>
+        <v>11</v>
+      </c>
+      <c r="C27" s="19" t="inlineStr">
+        <is>
+          <t>165</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
         <is>
-          <t>5:33:40</t>
+          <t>1:44:19</t>
         </is>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>4:15:19</t>
+          <t>31:25</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>1:00:05</t>
+          <t>9:23</t>
         </is>
       </c>
       <c r="G27" s="3" t="inlineStr">
@@ -2894,26 +2894,26 @@
       </c>
       <c r="H27" s="3" t="inlineStr">
         <is>
-          <t>22:36</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I27" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>4:21</t>
         </is>
       </c>
       <c r="J27" s="3" t="inlineStr">
         <is>
-          <t>0:01</t>
-        </is>
-      </c>
-      <c r="K27" s="21" t="inlineStr">
-        <is>
-          <t>4.84</t>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="K27" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
         </is>
       </c>
       <c r="L27" s="21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M27" s="15" t="n"/>
       <c r="P27" s="15" t="n"/>
@@ -2922,30 +2922,30 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>Смертина София Сергеевна</t>
+          <t>Сонин Владимир Викторович</t>
         </is>
       </c>
       <c r="B28" s="18" t="n">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C28" s="22" t="inlineStr">
         <is>
-          <t>265</t>
+          <t>315</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
         <is>
-          <t>1:59:48</t>
+          <t>4:37:39</t>
         </is>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>1:07:55</t>
+          <t>3:53:31</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t>9:17</t>
+          <t>9:47</t>
         </is>
       </c>
       <c r="G28" s="3" t="inlineStr">
@@ -2955,12 +2955,12 @@
       </c>
       <c r="H28" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>12:13</t>
         </is>
       </c>
       <c r="I28" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>4:54</t>
         </is>
       </c>
       <c r="J28" s="3" t="inlineStr">
@@ -2968,13 +2968,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K28" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L28" s="24" t="n">
-        <v>1</v>
+      <c r="K28" s="21" t="inlineStr">
+        <is>
+          <t>4.91</t>
+        </is>
+      </c>
+      <c r="L28" s="19" t="n">
+        <v>0</v>
       </c>
       <c r="M28" s="15" t="n"/>
       <c r="P28" s="15" t="n"/>
@@ -2983,30 +2983,30 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>Шаламова Дарья Сергеевна</t>
+          <t>Стаценко Юлия Валентиновна</t>
         </is>
       </c>
       <c r="B29" s="18" t="n">
-        <v>49</v>
-      </c>
-      <c r="C29" s="19" t="inlineStr">
-        <is>
-          <t>158</t>
+        <v>20</v>
+      </c>
+      <c r="C29" s="22" t="inlineStr">
+        <is>
+          <t>276</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
-          <t>2:50:01</t>
+          <t>2:30:05</t>
         </is>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>2:14:23</t>
+          <t>1:33:03</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>22:01</t>
+          <t>3:38</t>
         </is>
       </c>
       <c r="G29" s="3" t="inlineStr">
@@ -3016,7 +3016,7 @@
       </c>
       <c r="H29" s="3" t="inlineStr">
         <is>
-          <t>8:39</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I29" s="3" t="inlineStr">
@@ -3029,13 +3029,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K29" s="22" t="inlineStr">
-        <is>
-          <t>3.80</t>
-        </is>
-      </c>
-      <c r="L29" s="21" t="n">
-        <v>5</v>
+      <c r="K29" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L29" s="19" t="n">
+        <v>0</v>
       </c>
       <c r="M29" s="15" t="n"/>
       <c r="P29" s="15" t="n"/>
@@ -3044,30 +3044,30 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>Шамли Алина Алексеевна</t>
+          <t>Третьяков Даниел Павлович</t>
         </is>
       </c>
       <c r="B30" s="18" t="n">
-        <v>9</v>
-      </c>
-      <c r="C30" s="23" t="inlineStr">
-        <is>
-          <t>590</t>
+        <v>41</v>
+      </c>
+      <c r="C30" s="19" t="inlineStr">
+        <is>
+          <t>179</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
         <is>
-          <t>1:45:13</t>
+          <t>5:34:00</t>
         </is>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>1:29:07</t>
+          <t>2:04:02</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
         <is>
-          <t>31:53</t>
+          <t>3:24</t>
         </is>
       </c>
       <c r="G30" s="3" t="inlineStr">
@@ -3077,7 +3077,7 @@
       </c>
       <c r="H30" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>10:44</t>
         </is>
       </c>
       <c r="I30" s="3" t="inlineStr">
@@ -3090,42 +3090,42 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K30" s="21" t="inlineStr">
-        <is>
-          <t>4.20</t>
-        </is>
-      </c>
-      <c r="L30" s="19" t="n">
-        <v>0</v>
+      <c r="K30" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L30" s="24" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>Шартнер Елена Александровна</t>
+          <t>Ханнанова Елизавета Рустамовна</t>
         </is>
       </c>
       <c r="B31" s="18" t="n">
-        <v>29</v>
-      </c>
-      <c r="C31" s="21" t="inlineStr">
-        <is>
-          <t>232</t>
+        <v>15</v>
+      </c>
+      <c r="C31" s="23" t="inlineStr">
+        <is>
+          <t>432</t>
         </is>
       </c>
       <c r="D31" s="3" t="inlineStr">
         <is>
-          <t>3:42:38</t>
+          <t>1:59:25</t>
         </is>
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>1:55:47</t>
+          <t>1:48:57</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>4:28</t>
+          <t>1:05:50</t>
         </is>
       </c>
       <c r="G31" s="3" t="inlineStr">
@@ -3140,7 +3140,7 @@
       </c>
       <c r="I31" s="3" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J31" s="3" t="inlineStr">
@@ -3153,109 +3153,241 @@
           <t>5.00</t>
         </is>
       </c>
-      <c r="L31" s="21" t="n">
-        <v>4</v>
+      <c r="L31" s="19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
+          <t>Шаламова Дарья Сергеевна</t>
+        </is>
+      </c>
+      <c r="B32" s="18" t="n">
+        <v>37</v>
+      </c>
+      <c r="C32" s="21" t="inlineStr">
+        <is>
+          <t>213</t>
+        </is>
+      </c>
+      <c r="D32" s="3" t="inlineStr">
+        <is>
+          <t>2:53:27</t>
+        </is>
+      </c>
+      <c r="E32" s="3" t="inlineStr">
+        <is>
+          <t>2:16:51</t>
+        </is>
+      </c>
+      <c r="F32" s="3" t="inlineStr">
+        <is>
+          <t>8:42</t>
+        </is>
+      </c>
+      <c r="G32" s="3" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>7:09</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="K32" s="22" t="inlineStr">
+        <is>
+          <t>3.66</t>
+        </is>
+      </c>
+      <c r="L32" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="inlineStr">
+        <is>
+          <t>Шамли Алина Алексеевна</t>
+        </is>
+      </c>
+      <c r="B33" s="18" t="n">
+        <v>12</v>
+      </c>
+      <c r="C33" s="23" t="inlineStr">
+        <is>
+          <t>395</t>
+        </is>
+      </c>
+      <c r="D33" s="3" t="inlineStr">
+        <is>
+          <t>1:48:21</t>
+        </is>
+      </c>
+      <c r="E33" s="3" t="inlineStr">
+        <is>
+          <t>1:21:28</t>
+        </is>
+      </c>
+      <c r="F33" s="3" t="inlineStr">
+        <is>
+          <t>3:47:18</t>
+        </is>
+      </c>
+      <c r="G33" s="3" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="K33" s="21" t="inlineStr">
+        <is>
+          <t>4.33</t>
+        </is>
+      </c>
+      <c r="L33" s="21" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="inlineStr">
+        <is>
+          <t>Швачка Мария Юрьевна</t>
+        </is>
+      </c>
+      <c r="B34" s="18" t="n">
+        <v>31</v>
+      </c>
+      <c r="C34" s="22" t="inlineStr">
+        <is>
+          <t>275</t>
+        </is>
+      </c>
+      <c r="D34" s="3" t="inlineStr">
+        <is>
+          <t>9:17:39</t>
+        </is>
+      </c>
+      <c r="E34" s="3" t="inlineStr">
+        <is>
+          <t>2:23:36</t>
+        </is>
+      </c>
+      <c r="F34" s="3" t="inlineStr">
+        <is>
+          <t>44:37</t>
+        </is>
+      </c>
+      <c r="G34" s="3" t="inlineStr">
+        <is>
+          <t>28:38</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>21:34</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>7:12</t>
+        </is>
+      </c>
+      <c r="J34" s="3" t="inlineStr">
+        <is>
+          <t>1:45:12</t>
+        </is>
+      </c>
+      <c r="K34" s="21" t="inlineStr">
+        <is>
+          <t>4.92</t>
+        </is>
+      </c>
+      <c r="L34" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="inlineStr">
+        <is>
           <t>Шептунова Софья Денисовна</t>
         </is>
       </c>
-      <c r="B32" s="18" t="n">
-        <v>31</v>
-      </c>
-      <c r="C32" s="22" t="inlineStr">
-        <is>
-          <t>249</t>
-        </is>
-      </c>
-      <c r="D32" s="3" t="inlineStr">
-        <is>
-          <t>3:04:12</t>
-        </is>
-      </c>
-      <c r="E32" s="3" t="inlineStr">
-        <is>
-          <t>2:10:37</t>
-        </is>
-      </c>
-      <c r="F32" s="3" t="inlineStr">
-        <is>
-          <t>1:04</t>
-        </is>
-      </c>
-      <c r="G32" s="3" t="inlineStr">
-        <is>
-          <t>0:00</t>
-        </is>
-      </c>
-      <c r="H32" s="3" t="inlineStr">
-        <is>
-          <t>0:00</t>
-        </is>
-      </c>
-      <c r="I32" s="3" t="inlineStr">
-        <is>
-          <t>0:00</t>
-        </is>
-      </c>
-      <c r="J32" s="3" t="inlineStr">
-        <is>
-          <t>0:00</t>
-        </is>
-      </c>
-      <c r="K32" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L32" s="21" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="3" t="n"/>
-      <c r="B33" s="3" t="n"/>
-      <c r="C33" s="10" t="n"/>
-      <c r="D33" s="3" t="n"/>
-      <c r="E33" s="3" t="n"/>
-      <c r="F33" s="3" t="n"/>
-      <c r="G33" s="3" t="n"/>
-      <c r="H33" s="3" t="n"/>
-      <c r="I33" s="3" t="n"/>
-      <c r="J33" s="3" t="n"/>
-      <c r="K33" s="10" t="n"/>
-      <c r="L33" s="13" t="n"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="3" t="n"/>
-      <c r="B34" s="3" t="n"/>
-      <c r="C34" s="10" t="n"/>
-      <c r="D34" s="3" t="n"/>
-      <c r="E34" s="3" t="n"/>
-      <c r="F34" s="3" t="n"/>
-      <c r="G34" s="3" t="n"/>
-      <c r="H34" s="3" t="n"/>
-      <c r="I34" s="3" t="n"/>
-      <c r="J34" s="3" t="n"/>
-      <c r="K34" s="10" t="n"/>
-      <c r="L34" s="13" t="n"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="3" t="n"/>
-      <c r="B35" s="3" t="n"/>
-      <c r="C35" s="10" t="n"/>
-      <c r="D35" s="3" t="n"/>
-      <c r="E35" s="3" t="n"/>
-      <c r="F35" s="3" t="n"/>
-      <c r="G35" s="3" t="n"/>
-      <c r="H35" s="3" t="n"/>
-      <c r="I35" s="3" t="n"/>
-      <c r="J35" s="3" t="n"/>
-      <c r="K35" s="10" t="n"/>
-      <c r="L35" s="13" t="n"/>
+      <c r="B35" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="C35" s="21" t="inlineStr">
+        <is>
+          <t>209</t>
+        </is>
+      </c>
+      <c r="D35" s="3" t="inlineStr">
+        <is>
+          <t>3:09:00</t>
+        </is>
+      </c>
+      <c r="E35" s="3" t="inlineStr">
+        <is>
+          <t>1:39:31</t>
+        </is>
+      </c>
+      <c r="F35" s="3" t="inlineStr">
+        <is>
+          <t>2:29</t>
+        </is>
+      </c>
+      <c r="G35" s="3" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="I35" s="3" t="inlineStr">
+        <is>
+          <t>1:56</t>
+        </is>
+      </c>
+      <c r="J35" s="3" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="K35" s="21" t="inlineStr">
+        <is>
+          <t>4.33</t>
+        </is>
+      </c>
+      <c r="L35" s="21" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="n"/>

</xml_diff>

<commit_message>
work 1.4.1 coef in google excel
</commit_message>
<xml_diff>
--- a/files_samples/Статистика операторов с пропущенными.xlsx
+++ b/files_samples/Статистика операторов с пропущенными.xlsx
@@ -1318,7 +1318,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Четверг, 14.11.2024</t>
+          <t>Понедельник, 18.11.2024</t>
         </is>
       </c>
       <c r="B1" s="16" t="n"/>
@@ -1402,26 +1402,26 @@
         </is>
       </c>
       <c r="B3" s="18" t="n">
-        <v>27</v>
-      </c>
-      <c r="C3" s="20" t="inlineStr">
-        <is>
-          <t>109</t>
+        <v>14</v>
+      </c>
+      <c r="C3" s="19" t="inlineStr">
+        <is>
+          <t>152</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>7:34:00</t>
+          <t>5:55:56</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>57:42</t>
+          <t>42:13</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>57:52</t>
+          <t>1:29</t>
         </is>
       </c>
       <c r="G3" s="3" t="inlineStr">
@@ -1436,21 +1436,21 @@
       </c>
       <c r="I3" s="3" t="inlineStr">
         <is>
-          <t>5:43</t>
+          <t>0:29</t>
         </is>
       </c>
       <c r="J3" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>0:01</t>
         </is>
       </c>
       <c r="K3" s="22" t="inlineStr">
         <is>
-          <t>4.85</t>
+          <t>5.00</t>
         </is>
       </c>
       <c r="L3" s="19" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="M3" s="15" t="n"/>
       <c r="P3" s="15" t="n"/>
@@ -1463,41 +1463,41 @@
         </is>
       </c>
       <c r="B4" s="19" t="n">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C4" s="19" t="inlineStr">
         <is>
-          <t>179</t>
+          <t>160</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>7:03:20</t>
+          <t>6:35:26</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>4:09:22</t>
+          <t>4:18:28</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>34:35</t>
+          <t>34:32</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">
         <is>
-          <t>30:05</t>
+          <t>24:04</t>
         </is>
       </c>
       <c r="H4" s="3" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="I4" s="3" t="inlineStr">
         <is>
-          <t>1:46</t>
+          <t>1:58</t>
         </is>
       </c>
       <c r="J4" s="3" t="inlineStr">
@@ -1510,8 +1510,8 @@
           <t>5.00</t>
         </is>
       </c>
-      <c r="L4" s="24" t="n">
-        <v>1</v>
+      <c r="L4" s="21" t="n">
+        <v>2</v>
       </c>
       <c r="M4" s="15" t="n"/>
       <c r="P4" s="15" t="n"/>
@@ -1524,26 +1524,26 @@
         </is>
       </c>
       <c r="B5" s="18" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C5" s="23" t="inlineStr">
         <is>
-          <t>528</t>
+          <t>417</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>1:08:40</t>
+          <t>1:47:41</t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>9:18</t>
+          <t>1:02:54</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>11:29</t>
+          <t>0:29</t>
         </is>
       </c>
       <c r="G5" s="3" t="inlineStr">
@@ -1558,7 +1558,7 @@
       </c>
       <c r="I5" s="3" t="inlineStr">
         <is>
-          <t>3:12</t>
+          <t>11:54</t>
         </is>
       </c>
       <c r="J5" s="3" t="inlineStr">
@@ -1566,13 +1566,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K5" s="22" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="L5" s="21" t="n">
-        <v>2</v>
+      <c r="K5" s="21" t="inlineStr">
+        <is>
+          <t>4.00</t>
+        </is>
+      </c>
+      <c r="L5" s="19" t="n">
+        <v>0</v>
       </c>
       <c r="M5" s="15" t="n"/>
       <c r="P5" s="15" t="n"/>
@@ -1581,59 +1581,59 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Гарипова Лейсан Миневелиевна</t>
-        </is>
-      </c>
-      <c r="B6" s="19" t="n">
-        <v>77</v>
-      </c>
-      <c r="C6" s="22" t="inlineStr">
-        <is>
-          <t>297</t>
+          <t>Бахтиаров Глеб Русланович</t>
+        </is>
+      </c>
+      <c r="B6" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="C6" s="21" t="inlineStr">
+        <is>
+          <t>213</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>9:18:53</t>
+          <t>2:11:12</t>
         </is>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>6:25:53</t>
+          <t>1:40:35</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>1:38</t>
+          <t>6:25</t>
         </is>
       </c>
       <c r="G6" s="3" t="inlineStr">
         <is>
-          <t>28:23</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="H6" s="3" t="inlineStr">
         <is>
-          <t>11:34</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I6" s="3" t="inlineStr">
         <is>
-          <t>2:57</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J6" s="3" t="inlineStr">
         <is>
-          <t>48:09</t>
-        </is>
-      </c>
-      <c r="K6" s="21" t="inlineStr">
-        <is>
-          <t>4.97</t>
-        </is>
-      </c>
-      <c r="L6" s="21" t="n">
-        <v>6</v>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="K6" s="22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L6" s="19" t="n">
+        <v>0</v>
       </c>
       <c r="M6" s="15" t="n"/>
       <c r="P6" s="15" t="n"/>
@@ -1642,40 +1642,40 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Гарифуллин Булат Дамирович</t>
-        </is>
-      </c>
-      <c r="B7" s="18" t="n">
-        <v>21</v>
-      </c>
-      <c r="C7" s="19" t="inlineStr">
-        <is>
-          <t>186</t>
+          <t>Гарипова Лейсан Миневелиевна</t>
+        </is>
+      </c>
+      <c r="B7" s="20" t="n">
+        <v>121</v>
+      </c>
+      <c r="C7" s="21" t="inlineStr">
+        <is>
+          <t>209</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>2:24:51</t>
+          <t>10:00:33</t>
         </is>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>1:07:38</t>
+          <t>7:06:30</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>42:15</t>
+          <t>26:33</t>
         </is>
       </c>
       <c r="G7" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>30:18</t>
         </is>
       </c>
       <c r="H7" s="3" t="inlineStr">
         <is>
-          <t>7:00</t>
+          <t>1:51</t>
         </is>
       </c>
       <c r="I7" s="3" t="inlineStr">
@@ -1685,16 +1685,16 @@
       </c>
       <c r="J7" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>1:20:23</t>
         </is>
       </c>
       <c r="K7" s="21" t="inlineStr">
         <is>
-          <t>4.50</t>
-        </is>
-      </c>
-      <c r="L7" s="24" t="n">
-        <v>1</v>
+          <t>4.98</t>
+        </is>
+      </c>
+      <c r="L7" s="21" t="n">
+        <v>2</v>
       </c>
       <c r="M7" s="15" t="n"/>
       <c r="P7" s="15" t="n"/>
@@ -1703,45 +1703,45 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>Горных Ксения Сергеевна</t>
+          <t>Гарифуллин Булат Дамирович</t>
         </is>
       </c>
       <c r="B8" s="18" t="n">
-        <v>64</v>
-      </c>
-      <c r="C8" s="21" t="inlineStr">
-        <is>
-          <t>226</t>
+        <v>58</v>
+      </c>
+      <c r="C8" s="19" t="inlineStr">
+        <is>
+          <t>188</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>6:58:14</t>
+          <t>4:32:44</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>4:06:05</t>
+          <t>3:08:43</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>1:39:47</t>
+          <t>37:42</t>
         </is>
       </c>
       <c r="G8" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>28:33</t>
         </is>
       </c>
       <c r="H8" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>6:23</t>
         </is>
       </c>
       <c r="I8" s="3" t="inlineStr">
         <is>
-          <t>3:22</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J8" s="3" t="inlineStr">
@@ -1749,13 +1749,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K8" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
+      <c r="K8" s="21" t="inlineStr">
+        <is>
+          <t>4.68</t>
         </is>
       </c>
       <c r="L8" s="21" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M8" s="15" t="n"/>
       <c r="P8" s="15" t="n"/>
@@ -1764,30 +1764,30 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>Гребенюк Полина Максимовна</t>
+          <t>Горных Ксения Сергеевна</t>
         </is>
       </c>
       <c r="B9" s="18" t="n">
-        <v>55</v>
-      </c>
-      <c r="C9" s="19" t="inlineStr">
-        <is>
-          <t>178</t>
+        <v>51</v>
+      </c>
+      <c r="C9" s="21" t="inlineStr">
+        <is>
+          <t>203</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>5:48:35</t>
+          <t>4:59:47</t>
         </is>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>2:45:11</t>
+          <t>2:57:47</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>2:31</t>
+          <t>2:04:32</t>
         </is>
       </c>
       <c r="G9" s="3" t="inlineStr">
@@ -1797,12 +1797,12 @@
       </c>
       <c r="H9" s="3" t="inlineStr">
         <is>
-          <t>11:24</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I9" s="3" t="inlineStr">
         <is>
-          <t>2:13</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J9" s="3" t="inlineStr">
@@ -1812,11 +1812,11 @@
       </c>
       <c r="K9" s="21" t="inlineStr">
         <is>
-          <t>4.80</t>
-        </is>
-      </c>
-      <c r="L9" s="24" t="n">
-        <v>1</v>
+          <t>4.93</t>
+        </is>
+      </c>
+      <c r="L9" s="21" t="n">
+        <v>10</v>
       </c>
       <c r="M9" s="15" t="n"/>
       <c r="Q9" s="15" t="n"/>
@@ -1824,45 +1824,45 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>Джабраилова Елена Валерьевна</t>
-        </is>
-      </c>
-      <c r="B10" s="20" t="n">
-        <v>142</v>
+          <t>Гребенюк Полина Максимовна</t>
+        </is>
+      </c>
+      <c r="B10" s="18" t="n">
+        <v>62</v>
       </c>
       <c r="C10" s="19" t="inlineStr">
         <is>
-          <t>185</t>
+          <t>199</t>
         </is>
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>11:25:05</t>
+          <t>5:54:25</t>
         </is>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>7:29:17</t>
+          <t>3:27:45</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>1:09</t>
+          <t>3:54</t>
         </is>
       </c>
       <c r="G10" s="3" t="inlineStr">
         <is>
-          <t>33:54</t>
+          <t>0:02</t>
         </is>
       </c>
       <c r="H10" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>6:39</t>
         </is>
       </c>
       <c r="I10" s="3" t="inlineStr">
         <is>
-          <t>2:05</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J10" s="3" t="inlineStr">
@@ -1870,13 +1870,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K10" s="22" t="inlineStr">
-        <is>
-          <t>4.78</t>
-        </is>
-      </c>
-      <c r="L10" s="21" t="n">
-        <v>19</v>
+      <c r="K10" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L10" s="19" t="n">
+        <v>0</v>
       </c>
       <c r="M10" s="15" t="n"/>
       <c r="P10" s="15" t="n"/>
@@ -1885,30 +1885,30 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Довыдович Алиса Станиславовна</t>
-        </is>
-      </c>
-      <c r="B11" s="18" t="n">
-        <v>57</v>
-      </c>
-      <c r="C11" s="21" t="inlineStr">
-        <is>
-          <t>231</t>
+          <t>Джабраилова Елена Валерьевна</t>
+        </is>
+      </c>
+      <c r="B11" s="19" t="n">
+        <v>71</v>
+      </c>
+      <c r="C11" s="19" t="inlineStr">
+        <is>
+          <t>189</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>5:40:38</t>
+          <t>4:56:22</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>3:40:53</t>
+          <t>3:52:12</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>16:03</t>
+          <t>2:48</t>
         </is>
       </c>
       <c r="G11" s="3" t="inlineStr">
@@ -1923,7 +1923,7 @@
       </c>
       <c r="I11" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>2:15</t>
         </is>
       </c>
       <c r="J11" s="3" t="inlineStr">
@@ -1933,11 +1933,11 @@
       </c>
       <c r="K11" s="21" t="inlineStr">
         <is>
-          <t>4.55</t>
-        </is>
-      </c>
-      <c r="L11" s="19" t="n">
-        <v>0</v>
+          <t>4.81</t>
+        </is>
+      </c>
+      <c r="L11" s="23" t="n">
+        <v>24</v>
       </c>
       <c r="M11" s="15" t="n"/>
       <c r="P11" s="15" t="n"/>
@@ -1950,26 +1950,26 @@
         </is>
       </c>
       <c r="B12" s="18" t="n">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C12" s="20" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>122</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>1:34:51</t>
+          <t>1:57:11</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>1:37:12</t>
+          <t>2:11:18</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>10:28:54</t>
+          <t>10:07:27</t>
         </is>
       </c>
       <c r="G12" s="3" t="inlineStr">
@@ -1989,16 +1989,16 @@
       </c>
       <c r="J12" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
-        </is>
-      </c>
-      <c r="K12" s="21" t="inlineStr">
-        <is>
-          <t>4.72</t>
-        </is>
-      </c>
-      <c r="L12" s="24" t="n">
-        <v>1</v>
+          <t>0:01</t>
+        </is>
+      </c>
+      <c r="K12" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L12" s="21" t="n">
+        <v>5</v>
       </c>
       <c r="M12" s="15" t="n"/>
       <c r="P12" s="15" t="n"/>
@@ -2011,31 +2011,31 @@
         </is>
       </c>
       <c r="B13" s="18" t="n">
-        <v>8</v>
-      </c>
-      <c r="C13" s="20" t="inlineStr">
-        <is>
-          <t>99</t>
+        <v>4</v>
+      </c>
+      <c r="C13" s="21" t="inlineStr">
+        <is>
+          <t>202</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>8:36:51</t>
+          <t>1:31:09</t>
         </is>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>14:48</t>
+          <t>13:33</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>11:08</t>
+          <t>12:01</t>
         </is>
       </c>
       <c r="G13" s="3" t="inlineStr">
         <is>
-          <t>8:46</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="H13" s="3" t="inlineStr">
@@ -2053,9 +2053,9 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K13" s="22" t="inlineStr">
-        <is>
-          <t>0.00</t>
+      <c r="K13" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
         </is>
       </c>
       <c r="L13" s="19" t="n">
@@ -2068,30 +2068,30 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>Зиберт Ольга Николаевна</t>
+          <t>Исаева Екатерина Аркадьевна</t>
         </is>
       </c>
       <c r="B14" s="18" t="n">
-        <v>23</v>
-      </c>
-      <c r="C14" s="23" t="inlineStr">
-        <is>
-          <t>499</t>
+        <v>48</v>
+      </c>
+      <c r="C14" s="22" t="inlineStr">
+        <is>
+          <t>281</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>3:58:16</t>
+          <t>4:45:46</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>3:12:44</t>
+          <t>3:53:23</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>24:55</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="G14" s="3" t="inlineStr">
@@ -2106,7 +2106,7 @@
       </c>
       <c r="I14" s="3" t="inlineStr">
         <is>
-          <t>1:41</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J14" s="3" t="inlineStr">
@@ -2114,13 +2114,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K14" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L14" s="24" t="n">
-        <v>1</v>
+      <c r="K14" s="21" t="inlineStr">
+        <is>
+          <t>4.82</t>
+        </is>
+      </c>
+      <c r="L14" s="23" t="n">
+        <v>33</v>
       </c>
       <c r="M14" s="15" t="n"/>
       <c r="P14" s="15" t="n"/>
@@ -2133,26 +2133,26 @@
         </is>
       </c>
       <c r="B15" s="18" t="n">
-        <v>12</v>
-      </c>
-      <c r="C15" s="19" t="inlineStr">
-        <is>
-          <t>150</t>
+        <v>21</v>
+      </c>
+      <c r="C15" s="21" t="inlineStr">
+        <is>
+          <t>203</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>2:38:26</t>
+          <t>3:56:26</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>31:09</t>
+          <t>1:13:07</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>0:14</t>
+          <t>0:46</t>
         </is>
       </c>
       <c r="G15" s="3" t="inlineStr">
@@ -2167,7 +2167,7 @@
       </c>
       <c r="I15" s="3" t="inlineStr">
         <is>
-          <t>4:29</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J15" s="3" t="inlineStr">
@@ -2175,13 +2175,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K15" s="21" t="inlineStr">
-        <is>
-          <t>4.60</t>
-        </is>
-      </c>
-      <c r="L15" s="24" t="n">
-        <v>1</v>
+      <c r="K15" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L15" s="21" t="n">
+        <v>6</v>
       </c>
       <c r="M15" s="15" t="n"/>
       <c r="P15" s="15" t="n"/>
@@ -2190,30 +2190,30 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>Матылицкая Елена Юрьевна</t>
+          <t>Маркелов Сергей Алексеевич</t>
         </is>
       </c>
       <c r="B16" s="18" t="n">
-        <v>13</v>
-      </c>
-      <c r="C16" s="23" t="inlineStr">
-        <is>
-          <t>520</t>
+        <v>63</v>
+      </c>
+      <c r="C16" s="20" t="inlineStr">
+        <is>
+          <t>140</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>1:59:44</t>
+          <t>7:43:56</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>1:53:04</t>
+          <t>2:28:48</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>3:09</t>
+          <t>36:03</t>
         </is>
       </c>
       <c r="G16" s="3" t="inlineStr">
@@ -2223,7 +2223,7 @@
       </c>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>8:55</t>
         </is>
       </c>
       <c r="I16" s="3" t="inlineStr">
@@ -2233,12 +2233,12 @@
       </c>
       <c r="J16" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
-        </is>
-      </c>
-      <c r="K16" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
+          <t>1:09:12</t>
+        </is>
+      </c>
+      <c r="K16" s="21" t="inlineStr">
+        <is>
+          <t>4.81</t>
         </is>
       </c>
       <c r="L16" s="19" t="n">
@@ -2255,26 +2255,26 @@
         </is>
       </c>
       <c r="B17" s="18" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C17" s="19" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>179</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>3:53:58</t>
+          <t>4:02:29</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>3:06:54</t>
+          <t>2:53:01</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>30:30</t>
+          <t>11:44:20</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
@@ -2297,13 +2297,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K17" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L17" s="21" t="n">
-        <v>7</v>
+      <c r="K17" s="21" t="inlineStr">
+        <is>
+          <t>4.57</t>
+        </is>
+      </c>
+      <c r="L17" s="24" t="n">
+        <v>1</v>
       </c>
       <c r="M17" s="15" t="n"/>
       <c r="P17" s="15" t="n"/>
@@ -2316,26 +2316,26 @@
         </is>
       </c>
       <c r="B18" s="18" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C18" s="23" t="inlineStr">
         <is>
-          <t>558</t>
+          <t>388</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>1:59:52</t>
+          <t>2:04:25</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>1:53:04</t>
+          <t>1:57:38</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>12:47:11</t>
+          <t>0:31</t>
         </is>
       </c>
       <c r="G18" s="3" t="inlineStr">
@@ -2373,30 +2373,30 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Орищенко Юлия Геннадьевна</t>
+          <t>Обучение 1</t>
         </is>
       </c>
       <c r="B19" s="18" t="n">
-        <v>37</v>
-      </c>
-      <c r="C19" s="21" t="inlineStr">
-        <is>
-          <t>216</t>
+        <v>6</v>
+      </c>
+      <c r="C19" s="23" t="inlineStr">
+        <is>
+          <t>463</t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>4:37:24</t>
+          <t>59:02</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>2:21:16</t>
+          <t>53:17</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>2:58</t>
+          <t>51:07</t>
         </is>
       </c>
       <c r="G19" s="3" t="inlineStr">
@@ -2411,7 +2411,7 @@
       </c>
       <c r="I19" s="3" t="inlineStr">
         <is>
-          <t>1:36</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J19" s="3" t="inlineStr">
@@ -2419,13 +2419,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K19" s="21" t="inlineStr">
-        <is>
-          <t>4.42</t>
-        </is>
-      </c>
-      <c r="L19" s="23" t="n">
-        <v>33</v>
+      <c r="K19" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L19" s="21" t="n">
+        <v>9</v>
       </c>
       <c r="M19" s="15" t="n"/>
       <c r="P19" s="15" t="n"/>
@@ -2434,30 +2434,30 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Павликов Илья Сергеевич</t>
+          <t>Обучение 3</t>
         </is>
       </c>
       <c r="B20" s="18" t="n">
-        <v>2</v>
-      </c>
-      <c r="C20" s="22" t="inlineStr">
-        <is>
-          <t>315</t>
+        <v>15</v>
+      </c>
+      <c r="C20" s="23" t="inlineStr">
+        <is>
+          <t>342</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>2:24:00</t>
+          <t>1:38:21</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>13:36</t>
+          <t>1:28:53</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>14:27</t>
+          <t>45:56</t>
         </is>
       </c>
       <c r="G20" s="3" t="inlineStr">
@@ -2467,7 +2467,7 @@
       </c>
       <c r="H20" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>1:54</t>
         </is>
       </c>
       <c r="I20" s="3" t="inlineStr">
@@ -2480,13 +2480,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K20" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L20" s="19" t="n">
-        <v>0</v>
+      <c r="K20" s="21" t="inlineStr">
+        <is>
+          <t>4.66</t>
+        </is>
+      </c>
+      <c r="L20" s="21" t="n">
+        <v>3</v>
       </c>
       <c r="M20" s="15" t="n"/>
       <c r="P20" s="15" t="n"/>
@@ -2495,30 +2495,30 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Плетнёв Владислав Евгеньевич</t>
+          <t>Обучение ICL</t>
         </is>
       </c>
       <c r="B21" s="18" t="n">
-        <v>36</v>
-      </c>
-      <c r="C21" s="21" t="inlineStr">
-        <is>
-          <t>208</t>
+        <v>4</v>
+      </c>
+      <c r="C21" s="22" t="inlineStr">
+        <is>
+          <t>293</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>7:38:29</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>2:09:29</t>
+          <t>24:06</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>0:56</t>
+          <t>28:29</t>
         </is>
       </c>
       <c r="G21" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
       </c>
       <c r="H21" s="3" t="inlineStr">
         <is>
-          <t>27:17</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I21" s="3" t="inlineStr">
@@ -2541,13 +2541,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K21" s="21" t="inlineStr">
-        <is>
-          <t>4.93</t>
-        </is>
-      </c>
-      <c r="L21" s="21" t="n">
-        <v>6</v>
+      <c r="K21" s="22" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="L21" s="24" t="n">
+        <v>1</v>
       </c>
       <c r="M21" s="15" t="n"/>
       <c r="P21" s="15" t="n"/>
@@ -2556,30 +2556,30 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>Путко Екатерина Николаевна</t>
+          <t>Орищенко Юлия Геннадьевна</t>
         </is>
       </c>
       <c r="B22" s="18" t="n">
-        <v>10</v>
-      </c>
-      <c r="C22" s="23" t="inlineStr">
-        <is>
-          <t>353</t>
+        <v>50</v>
+      </c>
+      <c r="C22" s="21" t="inlineStr">
+        <is>
+          <t>226</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
         <is>
-          <t>2:47:10</t>
+          <t>5:21:53</t>
         </is>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>59:58</t>
+          <t>3:14:44</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>2:13:39</t>
+          <t>1:35:01</t>
         </is>
       </c>
       <c r="G22" s="3" t="inlineStr">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="I22" s="3" t="inlineStr">
         <is>
-          <t>8:36</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J22" s="3" t="inlineStr">
@@ -2602,13 +2602,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K22" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L22" s="21" t="n">
-        <v>2</v>
+      <c r="K22" s="21" t="inlineStr">
+        <is>
+          <t>4.78</t>
+        </is>
+      </c>
+      <c r="L22" s="23" t="n">
+        <v>23</v>
       </c>
       <c r="M22" s="15" t="n"/>
       <c r="P22" s="15" t="n"/>
@@ -2617,30 +2617,30 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Рыжкина Екатерина Михайловна</t>
+          <t>Павликов Илья Сергеевич</t>
         </is>
       </c>
       <c r="B23" s="18" t="n">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C23" s="21" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>205</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
-          <t>3:02:42</t>
+          <t>8:10:15</t>
         </is>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>1:56:04</t>
+          <t>33:10</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>19:52</t>
+          <t>2:04:33</t>
         </is>
       </c>
       <c r="G23" s="3" t="inlineStr">
@@ -2655,7 +2655,7 @@
       </c>
       <c r="I23" s="3" t="inlineStr">
         <is>
-          <t>2:04</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J23" s="3" t="inlineStr">
@@ -2663,9 +2663,9 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K23" s="21" t="inlineStr">
-        <is>
-          <t>4.83</t>
+      <c r="K23" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
         </is>
       </c>
       <c r="L23" s="19" t="n">
@@ -2678,30 +2678,30 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>Севостьянов Михаил Игоревич</t>
+          <t>Плетнёв Владислав Евгеньевич</t>
         </is>
       </c>
       <c r="B24" s="18" t="n">
-        <v>35</v>
-      </c>
-      <c r="C24" s="22" t="inlineStr">
-        <is>
-          <t>272</t>
+        <v>31</v>
+      </c>
+      <c r="C24" s="19" t="inlineStr">
+        <is>
+          <t>160</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
         <is>
-          <t>4:41:18</t>
+          <t>7:28:41</t>
         </is>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>2:43:16</t>
+          <t>1:27:01</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>2:40</t>
+          <t>52:57</t>
         </is>
       </c>
       <c r="G24" s="3" t="inlineStr">
@@ -2711,12 +2711,12 @@
       </c>
       <c r="H24" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>36:23</t>
         </is>
       </c>
       <c r="I24" s="3" t="inlineStr">
         <is>
-          <t>4:51</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J24" s="3" t="inlineStr">
@@ -2724,13 +2724,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K24" s="21" t="inlineStr">
-        <is>
-          <t>4.90</t>
-        </is>
-      </c>
-      <c r="L24" s="19" t="n">
-        <v>0</v>
+      <c r="K24" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L24" s="21" t="n">
+        <v>8</v>
       </c>
       <c r="M24" s="15" t="n"/>
       <c r="P24" s="15" t="n"/>
@@ -2739,30 +2739,30 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>Серова Юлия Владимировна</t>
+          <t>Путко Екатерина Николаевна</t>
         </is>
       </c>
       <c r="B25" s="18" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C25" s="23" t="inlineStr">
         <is>
-          <t>356</t>
+          <t>344</t>
         </is>
       </c>
       <c r="D25" s="3" t="inlineStr">
         <is>
-          <t>3:40:01</t>
+          <t>2:00:22</t>
         </is>
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>3:01:16</t>
+          <t>1:03:56</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>6:06</t>
+          <t>2:09:03</t>
         </is>
       </c>
       <c r="G25" s="3" t="inlineStr">
@@ -2772,7 +2772,7 @@
       </c>
       <c r="H25" s="3" t="inlineStr">
         <is>
-          <t>9:18</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I25" s="3" t="inlineStr">
@@ -2785,13 +2785,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K25" s="22" t="inlineStr">
+      <c r="K25" s="19" t="inlineStr">
         <is>
           <t>5.00</t>
         </is>
       </c>
-      <c r="L25" s="19" t="n">
-        <v>12</v>
+      <c r="L25" s="24" t="n">
+        <v>1</v>
       </c>
       <c r="M25" s="15" t="n"/>
       <c r="P25" s="15" t="n"/>
@@ -2800,30 +2800,30 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>Силин Егор Владимирович</t>
+          <t>Рыжкина Екатерина Михайловна</t>
         </is>
       </c>
       <c r="B26" s="18" t="n">
-        <v>27</v>
-      </c>
-      <c r="C26" s="23" t="inlineStr">
-        <is>
-          <t>365</t>
+        <v>38</v>
+      </c>
+      <c r="C26" s="22" t="inlineStr">
+        <is>
+          <t>308</t>
         </is>
       </c>
       <c r="D26" s="3" t="inlineStr">
         <is>
-          <t>4:11:28</t>
+          <t>4:03:27</t>
         </is>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>2:46:43</t>
+          <t>3:16:38</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>43:03</t>
+          <t>30:01</t>
         </is>
       </c>
       <c r="G26" s="3" t="inlineStr">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="H26" s="3" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>2:20</t>
         </is>
       </c>
       <c r="I26" s="3" t="inlineStr">
@@ -2861,30 +2861,30 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>Смертина София Сергеевна</t>
+          <t>Серова Юлия Владимировна</t>
         </is>
       </c>
       <c r="B27" s="18" t="n">
-        <v>11</v>
-      </c>
-      <c r="C27" s="19" t="inlineStr">
-        <is>
-          <t>165</t>
+        <v>40</v>
+      </c>
+      <c r="C27" s="22" t="inlineStr">
+        <is>
+          <t>275</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
         <is>
-          <t>1:44:19</t>
+          <t>3:42:34</t>
         </is>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>31:25</t>
+          <t>3:05:52</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>9:23</t>
+          <t>6:04</t>
         </is>
       </c>
       <c r="G27" s="3" t="inlineStr">
@@ -2894,12 +2894,12 @@
       </c>
       <c r="H27" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="I27" s="3" t="inlineStr">
         <is>
-          <t>4:21</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J27" s="3" t="inlineStr">
@@ -2913,7 +2913,7 @@
         </is>
       </c>
       <c r="L27" s="21" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M27" s="15" t="n"/>
       <c r="P27" s="15" t="n"/>
@@ -2922,30 +2922,30 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>Сонин Владимир Викторович</t>
+          <t>Смертина София Сергеевна</t>
         </is>
       </c>
       <c r="B28" s="18" t="n">
-        <v>44</v>
-      </c>
-      <c r="C28" s="22" t="inlineStr">
-        <is>
-          <t>315</t>
+        <v>10</v>
+      </c>
+      <c r="C28" s="19" t="inlineStr">
+        <is>
+          <t>188</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
         <is>
-          <t>4:37:39</t>
+          <t>1:53:09</t>
         </is>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>3:53:31</t>
+          <t>33:08</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t>9:47</t>
+          <t>4:34:41</t>
         </is>
       </c>
       <c r="G28" s="3" t="inlineStr">
@@ -2955,12 +2955,12 @@
       </c>
       <c r="H28" s="3" t="inlineStr">
         <is>
-          <t>12:13</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I28" s="3" t="inlineStr">
         <is>
-          <t>4:54</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J28" s="3" t="inlineStr">
@@ -2968,13 +2968,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K28" s="21" t="inlineStr">
-        <is>
-          <t>4.91</t>
-        </is>
-      </c>
-      <c r="L28" s="19" t="n">
-        <v>0</v>
+      <c r="K28" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L28" s="21" t="n">
+        <v>5</v>
       </c>
       <c r="M28" s="15" t="n"/>
       <c r="P28" s="15" t="n"/>
@@ -2983,30 +2983,30 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>Стаценко Юлия Валентиновна</t>
+          <t>Сонин Владимир Викторович</t>
         </is>
       </c>
       <c r="B29" s="18" t="n">
-        <v>20</v>
-      </c>
-      <c r="C29" s="22" t="inlineStr">
-        <is>
-          <t>276</t>
+        <v>51</v>
+      </c>
+      <c r="C29" s="21" t="inlineStr">
+        <is>
+          <t>240</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
-          <t>2:30:05</t>
+          <t>4:32:29</t>
         </is>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>1:33:03</t>
+          <t>3:26:54</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>3:38</t>
+          <t>13:26</t>
         </is>
       </c>
       <c r="G29" s="3" t="inlineStr">
@@ -3016,7 +3016,7 @@
       </c>
       <c r="H29" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>19:43</t>
         </is>
       </c>
       <c r="I29" s="3" t="inlineStr">
@@ -3029,9 +3029,9 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K29" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
+      <c r="K29" s="21" t="inlineStr">
+        <is>
+          <t>4.94</t>
         </is>
       </c>
       <c r="L29" s="19" t="n">
@@ -3048,26 +3048,26 @@
         </is>
       </c>
       <c r="B30" s="18" t="n">
-        <v>41</v>
-      </c>
-      <c r="C30" s="19" t="inlineStr">
-        <is>
-          <t>179</t>
+        <v>61</v>
+      </c>
+      <c r="C30" s="21" t="inlineStr">
+        <is>
+          <t>224</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
         <is>
-          <t>5:34:00</t>
+          <t>5:46:23</t>
         </is>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>2:04:02</t>
+          <t>3:50:44</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
         <is>
-          <t>3:24</t>
+          <t>12:14</t>
         </is>
       </c>
       <c r="G30" s="3" t="inlineStr">
@@ -3077,7 +3077,7 @@
       </c>
       <c r="H30" s="3" t="inlineStr">
         <is>
-          <t>10:44</t>
+          <t>20:25</t>
         </is>
       </c>
       <c r="I30" s="3" t="inlineStr">
@@ -3090,13 +3090,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K30" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L30" s="24" t="n">
-        <v>1</v>
+      <c r="K30" s="21" t="inlineStr">
+        <is>
+          <t>4.93</t>
+        </is>
+      </c>
+      <c r="L30" s="19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -3106,26 +3106,26 @@
         </is>
       </c>
       <c r="B31" s="18" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C31" s="23" t="inlineStr">
         <is>
-          <t>432</t>
+          <t>771</t>
         </is>
       </c>
       <c r="D31" s="3" t="inlineStr">
         <is>
-          <t>1:59:25</t>
+          <t>2:52:42</t>
         </is>
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>1:48:57</t>
+          <t>2:48:06</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>1:05:50</t>
+          <t>1:26:56</t>
         </is>
       </c>
       <c r="G31" s="3" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="H31" s="3" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>6:20</t>
         </is>
       </c>
       <c r="I31" s="3" t="inlineStr">
@@ -3148,13 +3148,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K31" s="19" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="L31" s="19" t="n">
-        <v>0</v>
+      <c r="K31" s="21" t="inlineStr">
+        <is>
+          <t>4.33</t>
+        </is>
+      </c>
+      <c r="L31" s="24" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -3164,26 +3164,26 @@
         </is>
       </c>
       <c r="B32" s="18" t="n">
-        <v>37</v>
-      </c>
-      <c r="C32" s="21" t="inlineStr">
-        <is>
-          <t>213</t>
+        <v>30</v>
+      </c>
+      <c r="C32" s="22" t="inlineStr">
+        <is>
+          <t>294</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>2:53:27</t>
+          <t>2:51:15</t>
         </is>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>2:16:51</t>
+          <t>2:30:29</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
-          <t>8:42</t>
+          <t>24:36</t>
         </is>
       </c>
       <c r="G32" s="3" t="inlineStr">
@@ -3193,7 +3193,7 @@
       </c>
       <c r="H32" s="3" t="inlineStr">
         <is>
-          <t>7:09</t>
+          <t>8:58</t>
         </is>
       </c>
       <c r="I32" s="3" t="inlineStr">
@@ -3206,9 +3206,9 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K32" s="22" t="inlineStr">
-        <is>
-          <t>3.66</t>
+      <c r="K32" s="21" t="inlineStr">
+        <is>
+          <t>4.50</t>
         </is>
       </c>
       <c r="L32" s="24" t="n">
@@ -3222,26 +3222,26 @@
         </is>
       </c>
       <c r="B33" s="18" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C33" s="23" t="inlineStr">
         <is>
-          <t>395</t>
+          <t>853</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
         <is>
-          <t>1:48:21</t>
+          <t>1:52:37</t>
         </is>
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>1:21:28</t>
+          <t>1:40:39</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>3:47:18</t>
+          <t>9:58</t>
         </is>
       </c>
       <c r="G33" s="3" t="inlineStr">
@@ -3264,67 +3264,67 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K33" s="21" t="inlineStr">
-        <is>
-          <t>4.33</t>
+      <c r="K33" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
         </is>
       </c>
       <c r="L33" s="21" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>Швачка Мария Юрьевна</t>
+          <t>Шартнер Елена Александровна</t>
         </is>
       </c>
       <c r="B34" s="18" t="n">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C34" s="22" t="inlineStr">
         <is>
-          <t>275</t>
+          <t>337</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
         <is>
-          <t>9:17:39</t>
+          <t>1:08:28</t>
         </is>
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>2:23:36</t>
+          <t>1:02:40</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
         <is>
-          <t>44:37</t>
+          <t>2:51</t>
         </is>
       </c>
       <c r="G34" s="3" t="inlineStr">
         <is>
-          <t>28:38</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="H34" s="3" t="inlineStr">
         <is>
-          <t>21:34</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="I34" s="3" t="inlineStr">
         <is>
-          <t>7:12</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J34" s="3" t="inlineStr">
         <is>
-          <t>1:45:12</t>
-        </is>
-      </c>
-      <c r="K34" s="21" t="inlineStr">
-        <is>
-          <t>4.92</t>
+          <t>0:00</t>
+        </is>
+      </c>
+      <c r="K34" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
         </is>
       </c>
       <c r="L34" s="24" t="n">
@@ -3334,30 +3334,30 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>Шептунова Софья Денисовна</t>
+          <t>Швачка Мария Юрьевна</t>
         </is>
       </c>
       <c r="B35" s="18" t="n">
-        <v>28</v>
-      </c>
-      <c r="C35" s="21" t="inlineStr">
-        <is>
-          <t>209</t>
+        <v>5</v>
+      </c>
+      <c r="C35" s="23" t="inlineStr">
+        <is>
+          <t>358</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
-          <t>3:09:00</t>
+          <t>1:39:17</t>
         </is>
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>1:39:31</t>
+          <t>30:02</t>
         </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>2:29</t>
+          <t>35:40</t>
         </is>
       </c>
       <c r="G35" s="3" t="inlineStr">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="I35" s="3" t="inlineStr">
         <is>
-          <t>1:56</t>
+          <t>0:00</t>
         </is>
       </c>
       <c r="J35" s="3" t="inlineStr">
@@ -3380,13 +3380,13 @@
           <t>0:00</t>
         </is>
       </c>
-      <c r="K35" s="21" t="inlineStr">
-        <is>
-          <t>4.33</t>
-        </is>
-      </c>
-      <c r="L35" s="21" t="n">
-        <v>2</v>
+      <c r="K35" s="19" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="L35" s="19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">

</xml_diff>